<commit_message>
FEAT (Compilation template) Minor fixes
Minor fixes to a few entries (e.g. missing DP week, missing proper week number, etc.)
</commit_message>
<xml_diff>
--- a/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
+++ b/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="1858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="1870">
   <si>
     <t>Subject</t>
   </si>
@@ -9316,34 +9316,6 @@
 * Duplicates the first lesson at the Eucharist. The reading from Year 2 may be substituted.</t>
   </si>
   <si>
-    <t>Week of Easter
-Thursday of Easter week
-(Maelrubha of Applecross, Abbot, 722 [6] White)
-EUCHARIST
-Acts 3:11-26
-Psalm 8 or 114
-Luke 24:36b-48
-DAILY PRAYER: New Life: The Lord
-Ezekiel 37:1-14
-Acts 3:11-26* or 1 Corinthians 15:41-50
-John 15:12-27
-* Duplicates the first lesson at the Eucharist. The reading from Year 2 may be substituted.</t>
-  </si>
-  <si>
-    <t>Week of Easter
-Friday of Easter week
-(Anselm of Canterbury, Bishop and Teacher of the Faith, 1109 [6] White)
-EUCHARIST
-Acts 4:1-12
-Psalm 116:1-8
-John 21:1-14
-DAILY PRAYER: New Life: The Lord
-Daniel 12:1-4, 13
-Acts 4:1-12* or 1 Corinthians 15:51-58
-John 16:1-15
-* Duplicates the first lesson at the Eucharist. The reading from Year 2 may be substituted.</t>
-  </si>
-  <si>
     <t>Second Sunday of Easter [1] White; SPB First Sunday after Easter
 (Ordination of the Rt Revd Dr Gregor Duncan, Bishop of Glasgow and Galloway, 2010)
 EUCHARIST
@@ -9609,36 +9581,6 @@
 John 7:53 - 8:11</t>
   </si>
   <si>
-    <t>The Remaining Days of Christmas
-John Wycliffe, Priest, 1384 [6] White
-31 December (Hogmanay)
-DAILY EUCHARIST (White)
-1 John 2:18-21
-Psalm 96:1-2, 11-13
-John 1:1-18
-DAILY PRAYER: Incarnation 
-Morning:
-Isaiah 26:1-9
-2 Corinthians 5:16 - 6:2
-John 8:12-19
-Evening:
-Isaiah 65:15b-25
-Revelation 21:1-6</t>
-  </si>
-  <si>
-    <t>Week of Christmas 2
-Seraphim of Sarov, 1833 [6] White
-02 January
-DAILY EUCHARIST (White)
-1 John 1:22-29
-Psalm 98:1-5
-John 1:19-28
-DAILY PRAYER: Incarnation 
-Genesis 12:1-7
-Hebrews 11:1-12
-John 6:35-42, 48-51</t>
-  </si>
-  <si>
     <t>Week of Christmas 2
 Tuesday after the First Sunday after Christmas
 3 January
@@ -9663,23 +9605,6 @@
 Exodus 3:1-12
 Hebrews 11:23-31
 John 14:6-14</t>
-  </si>
-  <si>
-    <t>Week of Christmas 2
-Thursday after the First Sunday after Christmas
-5 January
-DAILY EUCHARIST (White)
-1 John 3:11-18
-Psalm 100
-John 1:43-51
-DAILY PRAYER: Incarnation 
-Morning:
-Joshua 1:1-9
-Hebrews 11:32 - 12:2
-John 15:1-16
-Evening:
-Isaiah 66:18-22
-Romans 15:7-13</t>
   </si>
   <si>
     <t>Saturday after the Epiphany</t>
@@ -10357,22 +10282,6 @@
 Deuteronomy 16:18-20; 17:14-20
 2 Corinthians 8:1-16
 Luke 18:1-8</t>
-  </si>
-  <si>
-    <t>Week of Advent 1
-Andrew, Apostle, Patron of Scotland [4] Red
-Wednesday after First Sunday of Advent
-EUCHARIST
-Deuteronomy 30:11-14 or Isaiah 52:7-10
-Psalm 19:1-6
-Romans 10:(8b-11), 12-18
-Matthew 4:18-22
-MORNING PRAYER: Festivals
-Isaiah 49:1-6
-1 Corinthians 4:1-16
-EVENING PRAYER: Festivals
-Isaiah 55:1-5
-John 1:35-42</t>
   </si>
   <si>
     <t>Saturday after Fourth Sunday after Epiphany (Consecration of the Rt Revd Kevin Pearson, Bishop of Argyll and the Isles, 2011)</t>
@@ -10554,31 +10463,6 @@
 John 19:25-27</t>
   </si>
   <si>
-    <t>Thomas, Apostle [4] Red (if not kept on 3 July)
-EUCHARIST
-Habakkuk 2:1-4
-Psalm 31:1-6
-Hebrews 10:35 - 11:1 or Ephesians 2:19-22
-John 20:24-29
-MORNING PRAYER: Festivals
-Job 42:1-6
-1 Peter 1:3-9
-EVENING PRAYER: Festivals
-Isaiah 43:8-13
-John 14:1-7
----
-Week of Advent 4
-21 December
-DAILY EUCHARIST (Violet)
-Song of Solomon 2:8-14 or Zephaniah 3:14-18a
-Psalm 33:1-5, 20-22
-Luke 1:39-45
-DAILY PRAYER: Anticipation 
-Isaiah 28:9-22
-Revelation 21:9-21
-Luke 1:26-38</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kentigern (or Mungo), Bishop c.603 [4] White
 EUCHARIST
 Isaiah 52:7-10
@@ -10922,20 +10806,6 @@
 Deuteronomy 30:1-10
 2 Corinthians 10:1-18
 Luke 18:31-43
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week of Proper 10 (if after Pentecost) [3] Green
-John Skinner, Priest, 1807, and John Skinner, Bishop, 1816 [6] White (translated from 12 June)
-Tuesday after Pentecost 1
-DAILY EUCHARIST
-2 Corinthians 1:18-22
-Psalm 119:129-136
-Matthew 5:13-16
-DAILY PRAYER: Week B
-Deuteronomy 30:11-20
-2 Corinthians 11:1-21a
-Luke 19:1-10
 </t>
   </si>
   <si>
@@ -13305,33 +13175,6 @@
   </si>
   <si>
     <t>Week of Proper 32 [3] Green
-REMEMBRANCE SUNDAY
-Job 19:21-27
-Psalm 90
-1 Corinthians 15:51-57
-John 6:37-40
----
-EUCHARIST
-Continuous:
-Joshua 24:1-3a, 14-25
-Psalm 78:1-7
-1 Thessalonians 4:13-18
-Matthew 25:1-13
-Thematic:
-Wisdom of Solomon 6:12-16 or Amos 5:18-24
-Psalm 70 or Wisdom of Solomon 6:17-20
-1 Thessalonians 4:13-18
-Matthew 25:1-13
-DAILY PRAYER: Week D
-Judges 7:2-22
-Romans 8:31-39
-John 15:9-17
-ALTERNATIVE PSALMS
-Morning: Psalm 82
-Evening: Psalm 46</t>
-  </si>
-  <si>
-    <t>Week of Proper 32 [3] Green
 Machar, Bishop, c.600 [6] White (translated from 12 November)
 Monday after Pentecost 23
 DAILY EUCHARIST
@@ -13518,8 +13361,435 @@
 Matthew 18:21-35</t>
   </si>
   <si>
-    <t>The Last Sunday after Pentecost (Christ the King) [3] White or Red (The Sunday before Advent)
-Week of Proper 34
+    <t>Week of Proper 34 [3] (Green)
+Monday after the Last Sunday after Pentecost
+DAILY EUCHARIST
+Daniel 1:1-20
+Psalm 24:1-6
+Luke 21:1-4
+DAILY PRAYER: Week B
+Joel 3:1-2, 9-17
+1 Peter 1:1-12
+Matthew 19:1-12</t>
+  </si>
+  <si>
+    <t>Week of Proper 34 [3] (Green)
+Tuesday after the Last Sunday after Pentecost
+DAILY EUCHARIST
+Daniel 2:31-45
+Psalm 96
+Luke 21:5-9
+DAILY PRAYER: Week B
+Nahum 1:1-13
+1 Peter 1:13-25
+Matthew 19:13-22</t>
+  </si>
+  <si>
+    <t>Week of Proper 34 [3] (Green)
+Wednesday after the Last Sunday after Pentecost
+DAILY EUCHARIST
+Daniel 5:1-6, 13-28
+Psalm 98
+Luke 21:10-19
+DAILY PRAYER: Week B
+Obadiah 15-21
+1 Peter 2:1-10
+Matthew 19:23-30</t>
+  </si>
+  <si>
+    <t>Week of Proper 34 [3] (Green)
+Charles de Foucauld, Priest and Hermit, 1916 [6] White
+Friday after the Last Sunday after Pentecost
+DAILY EUCHARIST
+Daniel 7:1-14
+Psalm 93
+Luke 21:29-33
+DAILY PRAYER: Week B
+Isaiah 24:14-23
+1 Peter 3:13 - 4:6
+Matthew 20:17-28</t>
+  </si>
+  <si>
+    <t>Week of Proper 34 [3] (Green)
+Nicholas Ferrar, Deacon, 1637 [6] White
+Saturday after the Last Sunday after Pentecost
+DAILY EUCHARIST
+Daniel 7:15-27
+Psalm 95:1-7
+Luke 21:34-36
+DAILY PRAYER: Week B
+Micah 7:11-20
+1 Peter 4:7-19
+Matthew 20:29-34</t>
+  </si>
+  <si>
+    <t>Week of Advent 1
+Andrew, Apostle, Patron of Scotland [4] Red
+EUCHARIST
+Deuteronomy 30:11-14 or Isaiah 52:7-10
+Psalm 19:1-6
+Romans 10:(8b-11), 12-18
+Matthew 4:18-22
+MORNING PRAYER: Festivals
+Isaiah 49:1-6
+1 Corinthians 4:1-16
+EVENING PRAYER: Festivals
+Isaiah 55:1-5
+John 1:35-42
+---
+Week of Advent 1
+Wednesday after First Sunday of Advent
+DAILY EUCHARIST (Violet)
+Isaiah 25:6-9 
+Psalm 23 
+Matthew 15:29-39 
+DAILY PRAYER: Anticipation 
+Isaiah 2:1-11
+1 Thessalonians 2:13-20
+Luke 20:19-26</t>
+  </si>
+  <si>
+    <t>Week of Advent 4
+Thomas, Apostle [4] Red (if not kept on 3 July)
+EUCHARIST
+Habakkuk 2:1-4
+Psalm 31:1-6
+Hebrews 10:35 - 11:1 or Ephesians 2:19-22
+John 20:24-29
+MORNING PRAYER: Festivals
+Job 42:1-6
+1 Peter 1:3-9
+EVENING PRAYER: Festivals
+Isaiah 43:8-13
+John 14:1-7
+---
+Week of Advent 4
+21 December
+DAILY EUCHARIST (Violet)
+Song of Solomon 2:8-14 or Zephaniah 3:14-18a
+Psalm 33:1-5, 20-22
+Luke 1:39-45
+DAILY PRAYER: Anticipation 
+Isaiah 28:9-22
+Revelation 21:9-21
+Luke 1:26-38</t>
+  </si>
+  <si>
+    <t>Christmas
+CHRISTMAS EVE [2] (24 December)
+DAILY EUCHARIST (Violet)
+2 Samuel 7:1-16
+Psalm 89:1-4, 19-29
+Luke 1:67-79
+MORNING PRAYER: Anticipation 
+Morning:
+Isaiah 35:1-10
+Revelation 22:12-17, 21
+Luke 1:67-80
+EVENING PRAYER: Anticipation 
+Isaiah 59:15b-21
+Philippians 2:5-11</t>
+  </si>
+  <si>
+    <t>The Remaining Days of Christmas
+Stephen, Deacon and Martyr [4] Red (26 December)
+DAILY EUCHARIST
+Jeremiah 26:1-9, 12-15
+Psalm 31:1-7, 16
+Acts 6:8 - 7:2a, 51c-60
+Matthew 23:34-39
+MORNING PRAYER: Incarnation/Festivals
+2 Chronicles 24:17-22
+Acts 6:1-7
+EVENING PRAYER: Incarnation/Festivals
+Wisdom of Solomon 4:7-15
+Acts 7:59 - 8:8</t>
+  </si>
+  <si>
+    <t>The Remaining Days of Christmas
+John, Apostle and Evangelist [4] White (27 December)
+DAILY EUCHARIST
+Genesis 1 or Genesis 1:1-5, 12-19
+Psalm 92:1-2, 11-14
+1 John 1:1-9
+John 20:1-8
+MORNING PRAYER: Incarnation/Festivals
+Proverbs 8:22-30
+John 13:20-35
+EVENING PRAYER: Incarnation/Festivals
+Isaiah 44:1-8
+1 John 5:1-12</t>
+  </si>
+  <si>
+    <t>The Remaining Days of Christmas
+The Holy Innocents [4] White (28 December)
+DAILY EUCHARIST
+Jeremiah 31:15-17
+Psalm 124
+Revelation 21:1-7
+Matthew 2:13-18
+MORNING PRAYER: Incarnation/Festivals
+Isaiah 49:13-23
+Matthew 18:1-14
+EVENING PRAYER: Incarnation/Festivals
+Isaiah 54:1-13
+Mark 10:13-16</t>
+  </si>
+  <si>
+    <t>The Remaining Days of Christmas
+John Wycliffe, Priest, 1384 [6] White
+31 December (Hogmanay)
+DAILY EUCHARIST (White)
+1 John 2:18-21
+Psalm 96:1-2, 11-13
+John 1:1-18
+MORNING PRAYER: Incarnation 
+Isaiah 26:1-9
+2 Corinthians 5:16 - 6:2
+John 8:12-19
+EVENING PRAYER: Incarnation 
+Isaiah 65:15b-25
+Revelation 21:1-6</t>
+  </si>
+  <si>
+    <t>Christmas
+CHRISTMAS DAY [1] White
+EUCHARIST
+Any of these propers may be used at midnight or during the day:  Those listed under C should be used at least once during the Christmas season:
+A
+Isaiah 9:2-7
+Psalm 96
+Titus 2:11-14
+Luke 2:1-14 (15-20) 
+B
+Isaiah 62:6-12
+Psalm 97
+Titus 3:4-7
+Luke 2: (1-7) 8-20
+C
+Isaiah 52:7-10
+Psalm 98
+Hebrews 1:1-4 (5-12) 
+John 1:1-14
+DAILY PRAYER: Incarnation 
+Zechariah 2:10-13
+1 John 4:7-16
+John 3:31-36
+"Happy Christmas! Thank you for using the SEC digital calendar."
+COLLECT
+O God,
+you have made this most holy night
+grow radiant with the brilliance of the true Light:
+grant that, as we have known the mystery of that Light on earth,
+so we may delight in him in heaven;
+through the same Jesus Christ, our Lord
+who lives and reigns with you,
+in the unity of the Holy Spirit,
+one God, world without end.
+Amen</t>
+  </si>
+  <si>
+    <t>Week of Advent 1
+FIRST SUNDAY OF ADVENT [1] Violet
+EUCHARIST
+Isaiah 2:1-5
+Psalm 122
+Romans 13:11-14
+Matthew 24:36-44
+DAILY PRAYER: Anticipation
+Isaiah 52:1-12
+Revelation 14:13 - 15:4
+Matthew 24:15-18
+ALTERNATIVE PSALMS
+Morning: Psalm 9
+Evening: Psalm 25
+Thank you for downloading and using the SEC digital calendar, I hope you find it useful.
+Love and blessings,
+Fr Gareth J M Saunders</t>
+  </si>
+  <si>
+    <t>Week of Christmas 2
+Seraphim of Sarov, 1833 [6] White
+2 January
+DAILY EUCHARIST (White)
+1 John 1:22-29
+Psalm 98:1-5
+John 1:19-28
+DAILY PRAYER: Incarnation 
+Genesis 12:1-7
+Hebrews 11:1-12
+John 6:35-42, 48-51</t>
+  </si>
+  <si>
+    <t>Week of Christmas 2
+THE NAMING OF JESUS [2] White
+1 January (New Year's Day)
+DAILY EUCHARIST
+Numbers 6:22-27
+Psalm 8
+Galatians 4:4-7 or Philippians 2:5-11
+Luke 2:15-21
+DAILY PRAYER: Incarnation/Festivals 
+Genesis 17:1-12a, 15-16
+Colossians 2:6-12
+John 16:23b-30
+"Happy new year! Lang may yer lum reek!"</t>
+  </si>
+  <si>
+    <t>Week of Christmas 2
+Thursday after the First Sunday after Christmas
+5 January
+DAILY EUCHARIST (White)
+1 John 3:11-18
+Psalm 100
+John 1:43-51
+MORNING PRAYER: Incarnation 
+Joshua 1:1-9
+Hebrews 11:32 - 12:2
+John 15:1-16
+EVENING PRAYER: Incarnation 
+Isaiah 66:18-22
+Romans 15:7-13</t>
+  </si>
+  <si>
+    <t>Epiphany
+THE EPIPHANY [1] White
+6 January
+EUCHARIST
+1 Isaiah 60:1-6
+Psalm 72:1-7, 10-14
+Ephesians 3:1-12
+Matthew 2:1-12
+DAILY PRAYER: Incarnation 
+Isaiah 52:7-10
+Revelation 21:22-27
+Matthew 12:14-21</t>
+  </si>
+  <si>
+    <t>Week of the Beginning of Lent
+Monday after Sunday before Lent
+DAILY EUCHARIST (Green)
+Sirach 17:24-29
+Psalm 32:1-8
+Mark 10:17-27
+DAILY PRAYER: Week C
+Deuteronomy 6:10-15
+Hebrews 1:1-14
+John 1:1-18</t>
+  </si>
+  <si>
+    <t>Week of the Beginning of Lent
+Tuesday after Sunday before Lent
+DAILY EUCHARIST (Green)
+Sirach 35:1-12
+Psalm 50:7-15
+Mark 10:28-31
+DAILY PRAYER: Week C
+Deuteronomy 6:16-25
+Hebrews 2:1-10
+John 1:19-28</t>
+  </si>
+  <si>
+    <t>Week of Easter
+Wednesday of Easter week
+EUCHARIST
+Acts 3:1-10
+Psalm 105:1-9
+Luke 24:13-35
+DAILY PRAYER: New Life: The Lord
+Micah 7:7-15
+Acts 3:1-10* or 1 Corinthians 15:(29), 30-41
+John 15:1-11
+Matthew 28:1-16
+* Duplicates the first lesson at the Eucharist. The reading from Year 2 (1 Corinthians 15) may be substituted.</t>
+  </si>
+  <si>
+    <t>Week of Easter
+Thursday of Easter week
+(Maelrubha of Applecross, Abbot, 722 [6] White)
+EUCHARIST
+Acts 3:11-26
+Psalm 8 or 114
+Luke 24:36b-48
+DAILY PRAYER: New Life: The Lord
+Ezekiel 37:1-14
+Acts 3:11-26* or 1 Corinthians 15:41-50
+John 15:12-27
+* Duplicates the first lesson at the Eucharist. The reading from Year 2 (1 Corinthians 15) may be substituted.</t>
+  </si>
+  <si>
+    <t>Week of Easter
+Friday of Easter week
+(Anselm of Canterbury, Bishop and Teacher of the Faith, 1109 [6] White)
+EUCHARIST
+Acts 4:1-12
+Psalm 116:1-8
+John 21:1-14
+DAILY PRAYER: New Life: The Lord
+Daniel 12:1-4, 13
+Acts 4:1-12* or 1 Corinthians 15:51-58
+John 16:1-15
+* Duplicates the first lesson at the Eucharist. The reading from Year 2 (1 Corinthians 15) may be substituted.</t>
+  </si>
+  <si>
+    <t>Week of Easter
+Saturday of Easter week
+EUCHARIST
+Acts 4:13-21
+Psalm 118:1-4, 22-29
+Mark 16:9-15
+DAILY PRAYER: New Life: The Lord
+Isaiah 25:1-9
+Acts 4:13-21, (22-31)* or 2 Corinthians 4:16 - 5:10
+John 16:16-33
+* Duplicates the first lesson at the Eucharist. The reading from Year 2 (1 Corinthians 4) may be substituted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week of Proper 10 (if after Pentecost) [3] Green
+John Skinner, Priest, 1807, and John Skinner, Bishop, 1816 [6] White (translated from 12 June)
+Tuesday after Pentecost 1
+DAILY EUCHARIST
+2 Corinthians 1:18-22
+Psalm 119:129-136
+Matthew 5:13-16
+DAILY PRAYER: Week B
+Deuteronomy 30:11-20
+2 Corinthians 11:1-21a
+Luke 19:1-10
+</t>
+  </si>
+  <si>
+    <t>Week of Proper 32 [3] Green
+Remembrance Sunday
+EUCHARIST
+Job 19:21-27
+Psalm 90
+1 Corinthians 15:51-57
+John 6:37-40
+---
+Pentecost 23 [3] Green; SPB Trinity 22
+EUCHARIST
+Continuous:
+Joshua 24:1-3a, 14-25
+Psalm 78:1-7
+1 Thessalonians 4:13-18
+Matthew 25:1-13
+Thematic:
+Wisdom of Solomon 6:12-16 or Amos 5:18-24
+Psalm 70 or Wisdom of Solomon 6:17-20
+1 Thessalonians 4:13-18
+Matthew 25:1-13
+DAILY PRAYER: Week D
+Judges 7:2-22
+Romans 8:31-39
+John 15:9-17
+ALTERNATIVE PSALMS
+Morning: Psalm 82
+Evening: Psalm 46</t>
+  </si>
+  <si>
+    <t>Week of Proper 34 [3] (Green)
+The Last Sunday after Pentecost (Christ the King) [3] White or Red (The Sunday before Advent)
 EUCHARIST
 Continuous:
 Ezekiel 34:11-16, 20-24
@@ -13541,42 +13811,7 @@
   </si>
   <si>
     <t>Week of Proper 34 [3] (Green)
-Monday after the Last Sunday after Pentecost
-DAILY EUCHARIST
-Daniel 1:1-20
-Psalm 24:1-6
-Luke 21:1-4
-DAILY PRAYER: Week B
-Joel 3:1-2, 9-17
-1 Peter 1:1-12
-Matthew 19:1-12</t>
-  </si>
-  <si>
-    <t>Week of Proper 34 [3] (Green)
-Tuesday after the Last Sunday after Pentecost
-DAILY EUCHARIST
-Daniel 2:31-45
-Psalm 96
-Luke 21:5-9
-DAILY PRAYER: Week B
-Nahum 1:1-13
-1 Peter 1:13-25
-Matthew 19:13-22</t>
-  </si>
-  <si>
-    <t>Week of Proper 34 [3] (Green)
-Wednesday after the Last Sunday after Pentecost
-DAILY EUCHARIST
-Daniel 5:1-6, 13-28
-Psalm 98
-Luke 21:10-19
-DAILY PRAYER: Week B
-Obadiah 15-21
-1 Peter 2:1-10
-Matthew 19:23-30</t>
-  </si>
-  <si>
-    <t>Andrew, Apostle, Patron of Scotland [4] Red
+Andrew, Apostle, Patron of Scotland [4] Red
 EUCHARIST
 Deuteronomy 30:11-14 or Isaiah 52:7-10
 Psalm 19:1-6
@@ -13599,32 +13834,6 @@
 Zephaniah 3:1-13
 1 Peter 2:11-25
 Matthew 20:1-16</t>
-  </si>
-  <si>
-    <t>Week of Proper 34 [3] (Green)
-Charles de Foucauld, Priest and Hermit, 1916 [6] White
-Friday after the Last Sunday after Pentecost
-DAILY EUCHARIST
-Daniel 7:1-14
-Psalm 93
-Luke 21:29-33
-DAILY PRAYER: Week B
-Isaiah 24:14-23
-1 Peter 3:13 - 4:6
-Matthew 20:17-28</t>
-  </si>
-  <si>
-    <t>Week of Proper 34 [3] (Green)
-Nicholas Ferrar, Deacon, 1637 [6] White
-Saturday after the Last Sunday after Pentecost
-DAILY EUCHARIST
-Daniel 7:15-27
-Psalm 95:1-7
-Luke 21:34-36
-DAILY PRAYER: Week B
-Micah 7:11-20
-1 Peter 4:7-19
-Matthew 20:29-34</t>
   </si>
 </sst>
 </file>
@@ -33748,9 +33957,9 @@
   </sheetPr>
   <dimension ref="A1:E387"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D371" sqref="D371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33784,7 +33993,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>1519</v>
       </c>
@@ -33795,7 +34004,7 @@
         <v>547</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>1048</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -33826,7 +34035,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>964</v>
       </c>
@@ -33837,7 +34046,7 @@
         <v>175</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>1659</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -33851,7 +34060,7 @@
         <v>135</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -33865,7 +34074,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -33879,7 +34088,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -33907,7 +34116,7 @@
         <v>1542</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -33921,7 +34130,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -33935,7 +34144,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -33949,7 +34158,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>1667</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34033,7 +34242,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>1672</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34061,7 +34270,7 @@
         <v>556</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>1673</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -34075,7 +34284,7 @@
         <v>557</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>1674</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34103,7 +34312,7 @@
         <v>739</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34117,7 +34326,7 @@
         <v>559</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34131,7 +34340,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>1668</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34145,7 +34354,7 @@
         <v>741</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34159,7 +34368,7 @@
         <v>742</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34173,7 +34382,7 @@
         <v>15</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>1379</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34187,10 +34396,10 @@
         <v>16</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
         <v>941</v>
       </c>
@@ -34201,10 +34410,10 @@
         <v>17</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>1504</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
         <v>942</v>
       </c>
@@ -34215,10 +34424,10 @@
         <v>18</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
         <v>964</v>
       </c>
@@ -34229,7 +34438,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>1051</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34243,7 +34452,7 @@
         <v>20</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34257,10 +34466,10 @@
         <v>137</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>967</v>
       </c>
@@ -34271,10 +34480,10 @@
         <v>21</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>1519</v>
       </c>
@@ -34285,7 +34494,7 @@
         <v>22</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>1081</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34299,7 +34508,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>1602</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34313,7 +34522,7 @@
         <v>1544</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>1603</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34327,10 +34536,10 @@
         <v>1545</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
         <v>965</v>
       </c>
@@ -34341,10 +34550,10 @@
         <v>1546</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
         <v>966</v>
       </c>
@@ -34355,7 +34564,7 @@
         <v>24</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>1052</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34366,10 +34575,10 @@
         <v>42742</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>1606</v>
+        <v>1601</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="270" x14ac:dyDescent="0.25">
@@ -34411,7 +34620,7 @@
         <v>25</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>1608</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34425,7 +34634,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>1609</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34453,7 +34662,7 @@
         <v>138</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>1669</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34467,7 +34676,7 @@
         <v>139</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>1610</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34509,7 +34718,7 @@
         <v>27</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>1611</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34523,7 +34732,7 @@
         <v>28</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>1612</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34565,7 +34774,7 @@
         <v>29</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34607,7 +34816,7 @@
         <v>30</v>
       </c>
       <c r="D61" s="36" t="s">
-        <v>1614</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34621,7 +34830,7 @@
         <v>31</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>1670</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34635,7 +34844,7 @@
         <v>32</v>
       </c>
       <c r="D63" s="36" t="s">
-        <v>1615</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34649,7 +34858,7 @@
         <v>140</v>
       </c>
       <c r="D64" s="36" t="s">
-        <v>1616</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34663,7 +34872,7 @@
         <v>33</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>1617</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34691,7 +34900,7 @@
         <v>34</v>
       </c>
       <c r="D67" s="36" t="s">
-        <v>1618</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34705,10 +34914,10 @@
         <v>35</v>
       </c>
       <c r="D68" s="36" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="285" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
         <v>964</v>
       </c>
@@ -34719,7 +34928,7 @@
         <v>36</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>1620</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34733,7 +34942,7 @@
         <v>37</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>1671</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34747,7 +34956,7 @@
         <v>141</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>1621</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34758,7 +34967,7 @@
         <v>42770</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
       <c r="D72" s="36" t="s">
         <v>1547</v>
@@ -34789,7 +34998,7 @@
         <v>142</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>1622</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34845,7 +35054,7 @@
         <v>38</v>
       </c>
       <c r="D78" s="36" t="s">
-        <v>1623</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34901,7 +35110,7 @@
         <v>39</v>
       </c>
       <c r="D82" s="36" t="s">
-        <v>1624</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34915,7 +35124,7 @@
         <v>40</v>
       </c>
       <c r="D83" s="36" t="s">
-        <v>1625</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34943,7 +35152,7 @@
         <v>143</v>
       </c>
       <c r="D85" s="36" t="s">
-        <v>1626</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34957,7 +35166,7 @@
         <v>41</v>
       </c>
       <c r="D86" s="36" t="s">
-        <v>1627</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34985,7 +35194,7 @@
         <v>1548</v>
       </c>
       <c r="D88" s="37" t="s">
-        <v>1628</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35027,7 +35236,7 @@
         <v>43</v>
       </c>
       <c r="D91" s="37" t="s">
-        <v>1629</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35069,7 +35278,7 @@
         <v>944</v>
       </c>
       <c r="D94" s="37" t="s">
-        <v>1675</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35083,7 +35292,7 @@
         <v>796</v>
       </c>
       <c r="D95" s="36" t="s">
-        <v>1449</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35097,7 +35306,7 @@
         <v>582</v>
       </c>
       <c r="D96" s="36" t="s">
-        <v>1450</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35125,7 +35334,7 @@
         <v>144</v>
       </c>
       <c r="D98" s="37" t="s">
-        <v>1630</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35139,7 +35348,7 @@
         <v>45</v>
       </c>
       <c r="D99" s="37" t="s">
-        <v>1631</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35153,7 +35362,7 @@
         <v>46</v>
       </c>
       <c r="D100" s="37" t="s">
-        <v>1632</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35181,7 +35390,7 @@
         <v>47</v>
       </c>
       <c r="D102" s="36" t="s">
-        <v>1633</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35195,7 +35404,7 @@
         <v>48</v>
       </c>
       <c r="D103" s="36" t="s">
-        <v>1634</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -35209,7 +35418,7 @@
         <v>49</v>
       </c>
       <c r="D104" s="36" t="s">
-        <v>1635</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35237,7 +35446,7 @@
         <v>50</v>
       </c>
       <c r="D106" s="36" t="s">
-        <v>1636</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="300" x14ac:dyDescent="0.25">
@@ -35248,7 +35457,7 @@
         <v>42805</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>1637</v>
+        <v>1632</v>
       </c>
       <c r="D107" s="36" t="s">
         <v>1550</v>
@@ -35321,7 +35530,7 @@
         <v>145</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>1638</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -35335,7 +35544,7 @@
         <v>146</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>1661</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35349,7 +35558,7 @@
         <v>147</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>1639</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35377,7 +35586,7 @@
         <v>1551</v>
       </c>
       <c r="D116" s="36" t="s">
-        <v>1662</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35391,7 +35600,7 @@
         <v>150</v>
       </c>
       <c r="D117" s="36" t="s">
-        <v>1640</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35405,7 +35614,7 @@
         <v>151</v>
       </c>
       <c r="D118" s="36" t="s">
-        <v>1641</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35419,7 +35628,7 @@
         <v>1552</v>
       </c>
       <c r="D119" s="36" t="s">
-        <v>1642</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="300" x14ac:dyDescent="0.25">
@@ -35433,7 +35642,7 @@
         <v>51</v>
       </c>
       <c r="D120" s="36" t="s">
-        <v>1643</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -35447,7 +35656,7 @@
         <v>152</v>
       </c>
       <c r="D121" s="36" t="s">
-        <v>1676</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="345" x14ac:dyDescent="0.25">
@@ -35489,7 +35698,7 @@
         <v>52</v>
       </c>
       <c r="D124" s="36" t="s">
-        <v>1644</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35503,7 +35712,7 @@
         <v>544</v>
       </c>
       <c r="D125" s="36" t="s">
-        <v>1645</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35545,7 +35754,7 @@
         <v>153</v>
       </c>
       <c r="D128" s="36" t="s">
-        <v>1646</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="270" x14ac:dyDescent="0.25">
@@ -35657,7 +35866,7 @@
         <v>1539</v>
       </c>
       <c r="D136" s="36" t="s">
-        <v>1677</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35797,7 +36006,7 @@
         <v>611</v>
       </c>
       <c r="D146" s="36" t="s">
-        <v>1468</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -35811,7 +36020,7 @@
         <v>612</v>
       </c>
       <c r="D147" s="36" t="s">
-        <v>1560</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35825,7 +36034,7 @@
         <v>613</v>
       </c>
       <c r="D148" s="36" t="s">
-        <v>1561</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -35839,7 +36048,7 @@
         <v>614</v>
       </c>
       <c r="D149" s="36" t="s">
-        <v>1470</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -35850,10 +36059,10 @@
         <v>42848</v>
       </c>
       <c r="C150" s="34" t="s">
-        <v>1647</v>
+        <v>1642</v>
       </c>
       <c r="D150" s="36" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -35881,7 +36090,7 @@
         <v>61</v>
       </c>
       <c r="D152" s="37" t="s">
-        <v>1663</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35895,7 +36104,7 @@
         <v>62</v>
       </c>
       <c r="D153" s="37" t="s">
-        <v>1648</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -35937,7 +36146,7 @@
         <v>63</v>
       </c>
       <c r="D156" s="37" t="s">
-        <v>1649</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35965,7 +36174,7 @@
         <v>155</v>
       </c>
       <c r="D158" s="37" t="s">
-        <v>1664</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35979,7 +36188,7 @@
         <v>1537</v>
       </c>
       <c r="D159" s="37" t="s">
-        <v>1650</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36063,7 +36272,7 @@
         <v>156</v>
       </c>
       <c r="D165" s="37" t="s">
-        <v>1651</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36116,10 +36325,10 @@
         <v>42867</v>
       </c>
       <c r="C169" s="34" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="D169" s="37" t="s">
-        <v>1652</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36161,7 +36370,7 @@
         <v>65</v>
       </c>
       <c r="D172" s="37" t="s">
-        <v>1665</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36256,10 +36465,10 @@
         <v>42877</v>
       </c>
       <c r="C179" s="34" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="D179" s="37" t="s">
-        <v>1678</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="285" x14ac:dyDescent="0.25">
@@ -36270,10 +36479,10 @@
         <v>42878</v>
       </c>
       <c r="C180" s="34" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="D180" s="37" t="s">
-        <v>1679</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="345" x14ac:dyDescent="0.25">
@@ -36284,10 +36493,10 @@
         <v>42879</v>
       </c>
       <c r="C181" s="34" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="D181" s="37" t="s">
-        <v>1680</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="195" x14ac:dyDescent="0.25">
@@ -36315,7 +36524,7 @@
         <v>68</v>
       </c>
       <c r="D183" s="37" t="s">
-        <v>1653</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="210" x14ac:dyDescent="0.25">
@@ -36326,10 +36535,10 @@
         <v>42882</v>
       </c>
       <c r="C184" s="34" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="D184" s="37" t="s">
-        <v>1654</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="255" x14ac:dyDescent="0.25">
@@ -36385,7 +36594,7 @@
         <v>69</v>
       </c>
       <c r="D188" s="37" t="s">
-        <v>1666</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -36399,7 +36608,7 @@
         <v>158</v>
       </c>
       <c r="D189" s="37" t="s">
-        <v>1655</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -36427,7 +36636,7 @@
         <v>70</v>
       </c>
       <c r="D191" s="37" t="s">
-        <v>1681</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="240" x14ac:dyDescent="0.25">
@@ -36456,7 +36665,7 @@
         <v>72</v>
       </c>
       <c r="D193" s="36" t="s">
-        <v>1656</v>
+        <v>1651</v>
       </c>
       <c r="E193" s="20"/>
     </row>
@@ -36468,10 +36677,10 @@
         <v>42892</v>
       </c>
       <c r="C194" s="34" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="D194" s="36" t="s">
-        <v>1657</v>
+        <v>1652</v>
       </c>
       <c r="E194" s="20"/>
     </row>
@@ -36483,10 +36692,10 @@
         <v>42893</v>
       </c>
       <c r="C195" s="34" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="D195" s="36" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="E195" s="20"/>
     </row>
@@ -36501,7 +36710,7 @@
         <v>1522</v>
       </c>
       <c r="D196" s="36" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="E196" s="20"/>
     </row>
@@ -36513,10 +36722,10 @@
         <v>42895</v>
       </c>
       <c r="C197" s="41" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="D197" s="36" t="s">
-        <v>1682</v>
+        <v>1675</v>
       </c>
       <c r="E197" s="20"/>
     </row>
@@ -36528,10 +36737,10 @@
         <v>42896</v>
       </c>
       <c r="C198" s="34" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="D198" s="36" t="s">
-        <v>1683</v>
+        <v>1676</v>
       </c>
       <c r="E198" s="20"/>
     </row>
@@ -36561,11 +36770,11 @@
         <v>74</v>
       </c>
       <c r="D200" s="36" t="s">
-        <v>1684</v>
+        <v>1677</v>
       </c>
       <c r="E200" s="20"/>
     </row>
-    <row r="201" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A201" s="34" t="s">
         <v>942</v>
       </c>
@@ -36573,10 +36782,10 @@
         <v>42899</v>
       </c>
       <c r="C201" s="34" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="D201" s="36" t="s">
-        <v>1685</v>
+        <v>1866</v>
       </c>
       <c r="E201" s="20"/>
     </row>
@@ -36591,7 +36800,7 @@
         <v>76</v>
       </c>
       <c r="D202" s="36" t="s">
-        <v>1686</v>
+        <v>1678</v>
       </c>
       <c r="E202" s="20"/>
     </row>
@@ -36606,7 +36815,7 @@
         <v>842</v>
       </c>
       <c r="D203" s="24" t="s">
-        <v>1687</v>
+        <v>1679</v>
       </c>
       <c r="E203" s="20"/>
     </row>
@@ -36621,7 +36830,7 @@
         <v>841</v>
       </c>
       <c r="D204" s="36" t="s">
-        <v>1688</v>
+        <v>1680</v>
       </c>
       <c r="E204" s="20"/>
     </row>
@@ -36636,7 +36845,7 @@
         <v>645</v>
       </c>
       <c r="D205" s="36" t="s">
-        <v>1689</v>
+        <v>1681</v>
       </c>
       <c r="E205" s="20"/>
     </row>
@@ -36651,7 +36860,7 @@
         <v>646</v>
       </c>
       <c r="D206" s="36" t="s">
-        <v>1690</v>
+        <v>1682</v>
       </c>
       <c r="E206" s="20"/>
     </row>
@@ -36663,10 +36872,10 @@
         <v>42905</v>
       </c>
       <c r="C207" s="34" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="D207" s="36" t="s">
-        <v>1691</v>
+        <v>1683</v>
       </c>
       <c r="E207" s="20"/>
     </row>
@@ -36681,7 +36890,7 @@
         <v>160</v>
       </c>
       <c r="D208" s="36" t="s">
-        <v>1692</v>
+        <v>1684</v>
       </c>
       <c r="E208" s="20"/>
     </row>
@@ -36696,7 +36905,7 @@
         <v>648</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>1693</v>
+        <v>1685</v>
       </c>
       <c r="E209" s="20"/>
     </row>
@@ -36711,7 +36920,7 @@
         <v>159</v>
       </c>
       <c r="D210" s="36" t="s">
-        <v>1694</v>
+        <v>1686</v>
       </c>
       <c r="E210" s="20"/>
     </row>
@@ -36726,7 +36935,7 @@
         <v>649</v>
       </c>
       <c r="D211" s="36" t="s">
-        <v>1695</v>
+        <v>1687</v>
       </c>
       <c r="E211" s="20"/>
     </row>
@@ -36741,7 +36950,7 @@
         <v>78</v>
       </c>
       <c r="D212" s="36" t="s">
-        <v>1697</v>
+        <v>1689</v>
       </c>
       <c r="E212" s="20"/>
     </row>
@@ -36756,7 +36965,7 @@
         <v>650</v>
       </c>
       <c r="D213" s="36" t="s">
-        <v>1696</v>
+        <v>1688</v>
       </c>
       <c r="E213" s="20"/>
     </row>
@@ -36771,7 +36980,7 @@
         <v>80</v>
       </c>
       <c r="D214" s="36" t="s">
-        <v>1698</v>
+        <v>1690</v>
       </c>
       <c r="E214" s="20"/>
     </row>
@@ -36786,7 +36995,7 @@
         <v>81</v>
       </c>
       <c r="D215" s="36" t="s">
-        <v>1699</v>
+        <v>1691</v>
       </c>
       <c r="E215" s="20"/>
     </row>
@@ -36801,7 +37010,7 @@
         <v>82</v>
       </c>
       <c r="D216" s="36" t="s">
-        <v>1700</v>
+        <v>1692</v>
       </c>
       <c r="E216" s="20"/>
     </row>
@@ -36816,7 +37025,7 @@
         <v>83</v>
       </c>
       <c r="D217" s="36" t="s">
-        <v>1701</v>
+        <v>1693</v>
       </c>
       <c r="E217" s="20"/>
     </row>
@@ -36828,10 +37037,10 @@
         <v>42916</v>
       </c>
       <c r="C218" s="34" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="D218" s="36" t="s">
-        <v>1702</v>
+        <v>1694</v>
       </c>
       <c r="E218" s="20"/>
     </row>
@@ -36846,7 +37055,7 @@
         <v>84</v>
       </c>
       <c r="D219" s="36" t="s">
-        <v>1703</v>
+        <v>1695</v>
       </c>
       <c r="E219" s="20"/>
     </row>
@@ -36861,7 +37070,7 @@
         <v>651</v>
       </c>
       <c r="D220" s="36" t="s">
-        <v>1705</v>
+        <v>1697</v>
       </c>
       <c r="E220" s="20"/>
     </row>
@@ -36876,7 +37085,7 @@
         <v>85</v>
       </c>
       <c r="D221" s="36" t="s">
-        <v>1704</v>
+        <v>1696</v>
       </c>
       <c r="E221" s="20"/>
     </row>
@@ -36891,7 +37100,7 @@
         <v>853</v>
       </c>
       <c r="D222" s="36" t="s">
-        <v>1706</v>
+        <v>1698</v>
       </c>
       <c r="E222" s="20"/>
     </row>
@@ -36906,7 +37115,7 @@
         <v>854</v>
       </c>
       <c r="D223" s="36" t="s">
-        <v>1707</v>
+        <v>1699</v>
       </c>
       <c r="E223" s="20"/>
     </row>
@@ -36921,7 +37130,7 @@
         <v>161</v>
       </c>
       <c r="D224" s="36" t="s">
-        <v>1708</v>
+        <v>1700</v>
       </c>
       <c r="E224" s="20"/>
     </row>
@@ -36936,7 +37145,7 @@
         <v>97</v>
       </c>
       <c r="D225" s="36" t="s">
-        <v>1709</v>
+        <v>1701</v>
       </c>
       <c r="E225" s="20"/>
     </row>
@@ -36951,7 +37160,7 @@
         <v>653</v>
       </c>
       <c r="D226" s="36" t="s">
-        <v>1710</v>
+        <v>1702</v>
       </c>
       <c r="E226" s="20"/>
     </row>
@@ -36966,7 +37175,7 @@
         <v>654</v>
       </c>
       <c r="D227" s="36" t="s">
-        <v>1711</v>
+        <v>1703</v>
       </c>
       <c r="E227" s="20"/>
     </row>
@@ -36981,7 +37190,7 @@
         <v>859</v>
       </c>
       <c r="D228" s="36" t="s">
-        <v>1712</v>
+        <v>1704</v>
       </c>
       <c r="E228" s="20"/>
     </row>
@@ -36996,7 +37205,7 @@
         <v>86</v>
       </c>
       <c r="D229" s="36" t="s">
-        <v>1713</v>
+        <v>1705</v>
       </c>
       <c r="E229" s="20"/>
     </row>
@@ -37011,7 +37220,7 @@
         <v>87</v>
       </c>
       <c r="D230" s="36" t="s">
-        <v>1714</v>
+        <v>1706</v>
       </c>
       <c r="E230" s="20"/>
     </row>
@@ -37026,7 +37235,7 @@
         <v>657</v>
       </c>
       <c r="D231" s="36" t="s">
-        <v>1715</v>
+        <v>1707</v>
       </c>
       <c r="E231" s="20"/>
     </row>
@@ -37041,7 +37250,7 @@
         <v>658</v>
       </c>
       <c r="D232" s="36" t="s">
-        <v>1716</v>
+        <v>1708</v>
       </c>
       <c r="E232" s="20"/>
     </row>
@@ -37056,7 +37265,7 @@
         <v>860</v>
       </c>
       <c r="D233" s="36" t="s">
-        <v>1717</v>
+        <v>1709</v>
       </c>
       <c r="E233" s="20"/>
     </row>
@@ -37071,7 +37280,7 @@
         <v>659</v>
       </c>
       <c r="D234" s="36" t="s">
-        <v>1718</v>
+        <v>1710</v>
       </c>
       <c r="E234" s="20"/>
     </row>
@@ -37086,7 +37295,7 @@
         <v>861</v>
       </c>
       <c r="D235" s="36" t="s">
-        <v>1719</v>
+        <v>1711</v>
       </c>
       <c r="E235" s="20"/>
     </row>
@@ -37101,7 +37310,7 @@
         <v>660</v>
       </c>
       <c r="D236" s="36" t="s">
-        <v>1720</v>
+        <v>1712</v>
       </c>
       <c r="E236" s="20"/>
     </row>
@@ -37116,7 +37325,7 @@
         <v>661</v>
       </c>
       <c r="D237" s="36" t="s">
-        <v>1721</v>
+        <v>1713</v>
       </c>
       <c r="E237" s="20"/>
     </row>
@@ -37131,7 +37340,7 @@
         <v>662</v>
       </c>
       <c r="D238" s="36" t="s">
-        <v>1722</v>
+        <v>1714</v>
       </c>
       <c r="E238" s="20"/>
     </row>
@@ -37146,7 +37355,7 @@
         <v>88</v>
       </c>
       <c r="D239" s="36" t="s">
-        <v>1723</v>
+        <v>1715</v>
       </c>
       <c r="E239" s="20"/>
     </row>
@@ -37161,7 +37370,7 @@
         <v>89</v>
       </c>
       <c r="D240" s="36" t="s">
-        <v>1724</v>
+        <v>1716</v>
       </c>
       <c r="E240" s="20"/>
     </row>
@@ -37176,7 +37385,7 @@
         <v>665</v>
       </c>
       <c r="D241" s="36" t="s">
-        <v>1725</v>
+        <v>1717</v>
       </c>
       <c r="E241" s="20"/>
     </row>
@@ -37191,7 +37400,7 @@
         <v>666</v>
       </c>
       <c r="D242" s="36" t="s">
-        <v>1726</v>
+        <v>1718</v>
       </c>
       <c r="E242" s="20"/>
     </row>
@@ -37206,7 +37415,7 @@
         <v>90</v>
       </c>
       <c r="D243" s="36" t="s">
-        <v>1727</v>
+        <v>1719</v>
       </c>
       <c r="E243" s="20"/>
     </row>
@@ -37221,7 +37430,7 @@
         <v>91</v>
       </c>
       <c r="D244" s="36" t="s">
-        <v>1728</v>
+        <v>1720</v>
       </c>
       <c r="E244" s="20"/>
     </row>
@@ -37236,7 +37445,7 @@
         <v>667</v>
       </c>
       <c r="D245" s="36" t="s">
-        <v>1729</v>
+        <v>1721</v>
       </c>
       <c r="E245" s="20"/>
     </row>
@@ -37251,7 +37460,7 @@
         <v>668</v>
       </c>
       <c r="D246" s="36" t="s">
-        <v>1730</v>
+        <v>1722</v>
       </c>
       <c r="E246" s="20"/>
     </row>
@@ -37266,7 +37475,7 @@
         <v>92</v>
       </c>
       <c r="D247" s="36" t="s">
-        <v>1731</v>
+        <v>1723</v>
       </c>
       <c r="E247" s="20"/>
     </row>
@@ -37281,7 +37490,7 @@
         <v>669</v>
       </c>
       <c r="D248" s="36" t="s">
-        <v>1732</v>
+        <v>1724</v>
       </c>
       <c r="E248" s="20"/>
     </row>
@@ -37296,7 +37505,7 @@
         <v>94</v>
       </c>
       <c r="D249" s="36" t="s">
-        <v>1733</v>
+        <v>1725</v>
       </c>
       <c r="E249" s="20"/>
     </row>
@@ -37308,10 +37517,10 @@
         <v>42948</v>
       </c>
       <c r="C250" s="34" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="D250" s="36" t="s">
-        <v>1734</v>
+        <v>1726</v>
       </c>
       <c r="E250" s="20"/>
     </row>
@@ -37326,7 +37535,7 @@
         <v>866</v>
       </c>
       <c r="D251" s="36" t="s">
-        <v>1735</v>
+        <v>1727</v>
       </c>
       <c r="E251" s="20"/>
     </row>
@@ -37341,7 +37550,7 @@
         <v>867</v>
       </c>
       <c r="D252" s="36" t="s">
-        <v>1736</v>
+        <v>1728</v>
       </c>
       <c r="E252" s="20"/>
     </row>
@@ -37356,7 +37565,7 @@
         <v>868</v>
       </c>
       <c r="D253" s="36" t="s">
-        <v>1737</v>
+        <v>1729</v>
       </c>
       <c r="E253" s="20"/>
     </row>
@@ -37371,7 +37580,7 @@
         <v>95</v>
       </c>
       <c r="D254" s="36" t="s">
-        <v>1738</v>
+        <v>1730</v>
       </c>
       <c r="E254" s="20"/>
     </row>
@@ -37386,7 +37595,7 @@
         <v>96</v>
       </c>
       <c r="D255" s="36" t="s">
-        <v>1739</v>
+        <v>1731</v>
       </c>
       <c r="E255" s="20"/>
     </row>
@@ -37401,7 +37610,7 @@
         <v>673</v>
       </c>
       <c r="D256" s="36" t="s">
-        <v>1740</v>
+        <v>1732</v>
       </c>
       <c r="E256" s="20"/>
     </row>
@@ -37416,7 +37625,7 @@
         <v>98</v>
       </c>
       <c r="D257" s="36" t="s">
-        <v>1741</v>
+        <v>1733</v>
       </c>
       <c r="E257" s="20"/>
     </row>
@@ -37431,7 +37640,7 @@
         <v>99</v>
       </c>
       <c r="D258" s="36" t="s">
-        <v>1742</v>
+        <v>1734</v>
       </c>
       <c r="E258" s="20"/>
     </row>
@@ -37446,7 +37655,7 @@
         <v>162</v>
       </c>
       <c r="D259" s="36" t="s">
-        <v>1743</v>
+        <v>1735</v>
       </c>
       <c r="E259" s="20"/>
     </row>
@@ -37461,7 +37670,7 @@
         <v>100</v>
       </c>
       <c r="D260" s="36" t="s">
-        <v>1744</v>
+        <v>1736</v>
       </c>
       <c r="E260" s="20"/>
     </row>
@@ -37476,7 +37685,7 @@
         <v>101</v>
       </c>
       <c r="D261" s="36" t="s">
-        <v>1745</v>
+        <v>1737</v>
       </c>
       <c r="E261" s="20"/>
     </row>
@@ -37491,7 +37700,7 @@
         <v>675</v>
       </c>
       <c r="D262" s="36" t="s">
-        <v>1746</v>
+        <v>1738</v>
       </c>
       <c r="E262" s="20"/>
     </row>
@@ -37506,7 +37715,7 @@
         <v>1538</v>
       </c>
       <c r="D263" s="36" t="s">
-        <v>1747</v>
+        <v>1739</v>
       </c>
       <c r="E263" s="20"/>
     </row>
@@ -37521,7 +37730,7 @@
         <v>103</v>
       </c>
       <c r="D264" s="36" t="s">
-        <v>1748</v>
+        <v>1740</v>
       </c>
       <c r="E264" s="20"/>
     </row>
@@ -37533,10 +37742,10 @@
         <v>42963</v>
       </c>
       <c r="C265" s="34" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="D265" s="36" t="s">
-        <v>1749</v>
+        <v>1741</v>
       </c>
       <c r="E265" s="20"/>
     </row>
@@ -37551,7 +37760,7 @@
         <v>879</v>
       </c>
       <c r="D266" s="36" t="s">
-        <v>1750</v>
+        <v>1742</v>
       </c>
       <c r="E266" s="20"/>
     </row>
@@ -37566,7 +37775,7 @@
         <v>880</v>
       </c>
       <c r="D267" s="36" t="s">
-        <v>1751</v>
+        <v>1743</v>
       </c>
       <c r="E267" s="20"/>
     </row>
@@ -37581,7 +37790,7 @@
         <v>881</v>
       </c>
       <c r="D268" s="36" t="s">
-        <v>1752</v>
+        <v>1744</v>
       </c>
       <c r="E268" s="20"/>
     </row>
@@ -37596,7 +37805,7 @@
         <v>676</v>
       </c>
       <c r="D269" s="36" t="s">
-        <v>1753</v>
+        <v>1745</v>
       </c>
       <c r="E269" s="20"/>
     </row>
@@ -37611,7 +37820,7 @@
         <v>1530</v>
       </c>
       <c r="D270" s="36" t="s">
-        <v>1754</v>
+        <v>1746</v>
       </c>
       <c r="E270" s="20"/>
     </row>
@@ -37626,7 +37835,7 @@
         <v>678</v>
       </c>
       <c r="D271" s="36" t="s">
-        <v>1755</v>
+        <v>1747</v>
       </c>
       <c r="E271" s="20"/>
     </row>
@@ -37641,7 +37850,7 @@
         <v>679</v>
       </c>
       <c r="D272" s="36" t="s">
-        <v>1756</v>
+        <v>1748</v>
       </c>
       <c r="E272" s="20"/>
     </row>
@@ -37656,7 +37865,7 @@
         <v>163</v>
       </c>
       <c r="D273" s="36" t="s">
-        <v>1757</v>
+        <v>1749</v>
       </c>
       <c r="E273" s="20"/>
     </row>
@@ -37671,7 +37880,7 @@
         <v>164</v>
       </c>
       <c r="D274" s="36" t="s">
-        <v>1758</v>
+        <v>1750</v>
       </c>
       <c r="E274" s="20"/>
     </row>
@@ -37686,7 +37895,7 @@
         <v>681</v>
       </c>
       <c r="D275" s="36" t="s">
-        <v>1759</v>
+        <v>1751</v>
       </c>
       <c r="E275" s="20"/>
     </row>
@@ -37701,7 +37910,7 @@
         <v>682</v>
       </c>
       <c r="D276" s="36" t="s">
-        <v>1760</v>
+        <v>1752</v>
       </c>
       <c r="E276" s="20"/>
     </row>
@@ -37716,7 +37925,7 @@
         <v>165</v>
       </c>
       <c r="D277" s="36" t="s">
-        <v>1761</v>
+        <v>1753</v>
       </c>
       <c r="E277" s="20"/>
     </row>
@@ -37731,7 +37940,7 @@
         <v>105</v>
       </c>
       <c r="D278" s="36" t="s">
-        <v>1762</v>
+        <v>1754</v>
       </c>
       <c r="E278" s="20"/>
     </row>
@@ -37743,10 +37952,10 @@
         <v>42977</v>
       </c>
       <c r="C279" s="34" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="D279" s="36" t="s">
-        <v>1763</v>
+        <v>1755</v>
       </c>
       <c r="E279" s="20"/>
     </row>
@@ -37761,7 +37970,7 @@
         <v>106</v>
       </c>
       <c r="D280" s="36" t="s">
-        <v>1764</v>
+        <v>1756</v>
       </c>
       <c r="E280" s="20"/>
     </row>
@@ -37776,7 +37985,7 @@
         <v>886</v>
       </c>
       <c r="D281" s="36" t="s">
-        <v>1765</v>
+        <v>1757</v>
       </c>
       <c r="E281" s="20"/>
     </row>
@@ -37791,7 +38000,7 @@
         <v>107</v>
       </c>
       <c r="D282" s="36" t="s">
-        <v>1766</v>
+        <v>1758</v>
       </c>
       <c r="E282" s="20"/>
     </row>
@@ -37806,7 +38015,7 @@
         <v>684</v>
       </c>
       <c r="D283" s="36" t="s">
-        <v>1767</v>
+        <v>1759</v>
       </c>
       <c r="E283" s="20"/>
     </row>
@@ -37821,7 +38030,7 @@
         <v>108</v>
       </c>
       <c r="D284" s="36" t="s">
-        <v>1768</v>
+        <v>1760</v>
       </c>
       <c r="E284" s="20"/>
     </row>
@@ -37836,7 +38045,7 @@
         <v>685</v>
       </c>
       <c r="D285" s="36" t="s">
-        <v>1769</v>
+        <v>1761</v>
       </c>
       <c r="E285" s="20"/>
     </row>
@@ -37851,7 +38060,7 @@
         <v>889</v>
       </c>
       <c r="D286" s="36" t="s">
-        <v>1770</v>
+        <v>1762</v>
       </c>
       <c r="E286" s="20"/>
     </row>
@@ -37866,7 +38075,7 @@
         <v>890</v>
       </c>
       <c r="D287" s="36" t="s">
-        <v>1771</v>
+        <v>1763</v>
       </c>
       <c r="E287" s="20"/>
     </row>
@@ -37881,7 +38090,7 @@
         <v>109</v>
       </c>
       <c r="D288" s="36" t="s">
-        <v>1772</v>
+        <v>1764</v>
       </c>
       <c r="E288" s="20"/>
     </row>
@@ -37896,7 +38105,7 @@
         <v>687</v>
       </c>
       <c r="D289" s="36" t="s">
-        <v>1773</v>
+        <v>1765</v>
       </c>
       <c r="E289" s="20"/>
     </row>
@@ -37911,7 +38120,7 @@
         <v>688</v>
       </c>
       <c r="D290" s="36" t="s">
-        <v>1774</v>
+        <v>1766</v>
       </c>
       <c r="E290" s="20"/>
     </row>
@@ -37926,7 +38135,7 @@
         <v>689</v>
       </c>
       <c r="D291" s="36" t="s">
-        <v>1775</v>
+        <v>1767</v>
       </c>
       <c r="E291" s="20"/>
     </row>
@@ -37941,7 +38150,7 @@
         <v>891</v>
       </c>
       <c r="D292" s="36" t="s">
-        <v>1776</v>
+        <v>1768</v>
       </c>
       <c r="E292" s="20"/>
     </row>
@@ -37956,7 +38165,7 @@
         <v>110</v>
       </c>
       <c r="D293" s="36" t="s">
-        <v>1777</v>
+        <v>1769</v>
       </c>
       <c r="E293" s="20"/>
     </row>
@@ -37971,7 +38180,7 @@
         <v>166</v>
       </c>
       <c r="D294" s="36" t="s">
-        <v>1778</v>
+        <v>1770</v>
       </c>
       <c r="E294" s="20"/>
     </row>
@@ -37986,7 +38195,7 @@
         <v>692</v>
       </c>
       <c r="D295" s="36" t="s">
-        <v>1779</v>
+        <v>1771</v>
       </c>
       <c r="E295" s="20"/>
     </row>
@@ -38001,7 +38210,7 @@
         <v>111</v>
       </c>
       <c r="D296" s="36" t="s">
-        <v>1780</v>
+        <v>1772</v>
       </c>
       <c r="E296" s="20"/>
     </row>
@@ -38016,7 +38225,7 @@
         <v>694</v>
       </c>
       <c r="D297" s="36" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="E297" s="20"/>
     </row>
@@ -38031,7 +38240,7 @@
         <v>112</v>
       </c>
       <c r="D298" s="36" t="s">
-        <v>1782</v>
+        <v>1774</v>
       </c>
       <c r="E298" s="20"/>
     </row>
@@ -38046,7 +38255,7 @@
         <v>893</v>
       </c>
       <c r="D299" s="36" t="s">
-        <v>1783</v>
+        <v>1775</v>
       </c>
       <c r="E299" s="20"/>
     </row>
@@ -38061,7 +38270,7 @@
         <v>113</v>
       </c>
       <c r="D300" s="36" t="s">
-        <v>1784</v>
+        <v>1776</v>
       </c>
       <c r="E300" s="20"/>
     </row>
@@ -38076,7 +38285,7 @@
         <v>167</v>
       </c>
       <c r="D301" s="36" t="s">
-        <v>1785</v>
+        <v>1777</v>
       </c>
       <c r="E301" s="20"/>
     </row>
@@ -38088,10 +38297,10 @@
         <v>43000</v>
       </c>
       <c r="C302" s="34" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="D302" s="36" t="s">
-        <v>1786</v>
+        <v>1778</v>
       </c>
       <c r="E302" s="20"/>
     </row>
@@ -38103,10 +38312,10 @@
         <v>43001</v>
       </c>
       <c r="C303" s="34" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="D303" s="36" t="s">
-        <v>1787</v>
+        <v>1779</v>
       </c>
       <c r="E303" s="20"/>
     </row>
@@ -38121,7 +38330,7 @@
         <v>697</v>
       </c>
       <c r="D304" s="36" t="s">
-        <v>1788</v>
+        <v>1780</v>
       </c>
       <c r="E304" s="20"/>
     </row>
@@ -38136,7 +38345,7 @@
         <v>176</v>
       </c>
       <c r="D305" s="36" t="s">
-        <v>1789</v>
+        <v>1781</v>
       </c>
       <c r="E305" s="20"/>
     </row>
@@ -38151,7 +38360,7 @@
         <v>897</v>
       </c>
       <c r="D306" s="36" t="s">
-        <v>1790</v>
+        <v>1782</v>
       </c>
       <c r="E306" s="20"/>
     </row>
@@ -38166,7 +38375,7 @@
         <v>115</v>
       </c>
       <c r="D307" s="36" t="s">
-        <v>1791</v>
+        <v>1783</v>
       </c>
       <c r="E307" s="20"/>
     </row>
@@ -38181,7 +38390,7 @@
         <v>698</v>
       </c>
       <c r="D308" s="36" t="s">
-        <v>1792</v>
+        <v>1784</v>
       </c>
       <c r="E308" s="20"/>
     </row>
@@ -38196,7 +38405,7 @@
         <v>116</v>
       </c>
       <c r="D309" s="36" t="s">
-        <v>1793</v>
+        <v>1785</v>
       </c>
       <c r="E309" s="20"/>
     </row>
@@ -38211,7 +38420,7 @@
         <v>117</v>
       </c>
       <c r="D310" s="36" t="s">
-        <v>1794</v>
+        <v>1786</v>
       </c>
       <c r="E310" s="20"/>
     </row>
@@ -38226,7 +38435,7 @@
         <v>700</v>
       </c>
       <c r="D311" s="36" t="s">
-        <v>1795</v>
+        <v>1787</v>
       </c>
       <c r="E311" s="20"/>
     </row>
@@ -38238,10 +38447,10 @@
         <v>43010</v>
       </c>
       <c r="C312" s="34" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="D312" s="36" t="s">
-        <v>1796</v>
+        <v>1788</v>
       </c>
       <c r="E312" s="20"/>
     </row>
@@ -38256,7 +38465,7 @@
         <v>901</v>
       </c>
       <c r="D313" s="36" t="s">
-        <v>1797</v>
+        <v>1789</v>
       </c>
       <c r="E313" s="20"/>
     </row>
@@ -38271,7 +38480,7 @@
         <v>119</v>
       </c>
       <c r="D314" s="36" t="s">
-        <v>1798</v>
+        <v>1790</v>
       </c>
       <c r="E314" s="20"/>
     </row>
@@ -38286,7 +38495,7 @@
         <v>903</v>
       </c>
       <c r="D315" s="36" t="s">
-        <v>1799</v>
+        <v>1791</v>
       </c>
       <c r="E315" s="20"/>
     </row>
@@ -38301,7 +38510,7 @@
         <v>701</v>
       </c>
       <c r="D316" s="36" t="s">
-        <v>1800</v>
+        <v>1792</v>
       </c>
       <c r="E316" s="20"/>
     </row>
@@ -38316,7 +38525,7 @@
         <v>702</v>
       </c>
       <c r="D317" s="36" t="s">
-        <v>1801</v>
+        <v>1793</v>
       </c>
       <c r="E317" s="20"/>
     </row>
@@ -38328,10 +38537,10 @@
         <v>43016</v>
       </c>
       <c r="C318" s="34" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="D318" s="36" t="s">
-        <v>1802</v>
+        <v>1794</v>
       </c>
       <c r="E318" s="20"/>
     </row>
@@ -38343,10 +38552,10 @@
         <v>43017</v>
       </c>
       <c r="C319" s="34" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="D319" s="36" t="s">
-        <v>1803</v>
+        <v>1795</v>
       </c>
       <c r="E319" s="20"/>
     </row>
@@ -38361,7 +38570,7 @@
         <v>704</v>
       </c>
       <c r="D320" s="36" t="s">
-        <v>1804</v>
+        <v>1796</v>
       </c>
       <c r="E320" s="20"/>
     </row>
@@ -38376,7 +38585,7 @@
         <v>120</v>
       </c>
       <c r="D321" s="36" t="s">
-        <v>1805</v>
+        <v>1797</v>
       </c>
       <c r="E321" s="20"/>
     </row>
@@ -38391,7 +38600,7 @@
         <v>168</v>
       </c>
       <c r="D322" s="36" t="s">
-        <v>1806</v>
+        <v>1798</v>
       </c>
       <c r="E322" s="20"/>
     </row>
@@ -38403,10 +38612,10 @@
         <v>43021</v>
       </c>
       <c r="C323" s="34" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="D323" s="36" t="s">
-        <v>1807</v>
+        <v>1799</v>
       </c>
       <c r="E323" s="20"/>
     </row>
@@ -38421,7 +38630,7 @@
         <v>707</v>
       </c>
       <c r="D324" s="36" t="s">
-        <v>1808</v>
+        <v>1800</v>
       </c>
       <c r="E324" s="20"/>
     </row>
@@ -38436,7 +38645,7 @@
         <v>708</v>
       </c>
       <c r="D325" s="36" t="s">
-        <v>1809</v>
+        <v>1801</v>
       </c>
       <c r="E325" s="20"/>
     </row>
@@ -38448,10 +38657,10 @@
         <v>43024</v>
       </c>
       <c r="C326" s="34" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D326" s="36" t="s">
-        <v>1810</v>
+        <v>1802</v>
       </c>
       <c r="E326" s="20"/>
     </row>
@@ -38466,7 +38675,7 @@
         <v>122</v>
       </c>
       <c r="D327" s="36" t="s">
-        <v>1811</v>
+        <v>1803</v>
       </c>
       <c r="E327" s="20"/>
     </row>
@@ -38481,7 +38690,7 @@
         <v>123</v>
       </c>
       <c r="D328" s="36" t="s">
-        <v>1812</v>
+        <v>1804</v>
       </c>
       <c r="E328" s="20"/>
     </row>
@@ -38496,7 +38705,7 @@
         <v>169</v>
       </c>
       <c r="D329" s="36" t="s">
-        <v>1813</v>
+        <v>1805</v>
       </c>
       <c r="E329" s="20"/>
     </row>
@@ -38511,7 +38720,7 @@
         <v>710</v>
       </c>
       <c r="D330" s="36" t="s">
-        <v>1814</v>
+        <v>1806</v>
       </c>
       <c r="E330" s="20"/>
     </row>
@@ -38526,7 +38735,7 @@
         <v>909</v>
       </c>
       <c r="D331" s="36" t="s">
-        <v>1815</v>
+        <v>1807</v>
       </c>
       <c r="E331" s="20"/>
     </row>
@@ -38541,7 +38750,7 @@
         <v>711</v>
       </c>
       <c r="D332" s="36" t="s">
-        <v>1816</v>
+        <v>1808</v>
       </c>
       <c r="E332" s="20"/>
     </row>
@@ -38556,7 +38765,7 @@
         <v>1527</v>
       </c>
       <c r="D333" s="36" t="s">
-        <v>1817</v>
+        <v>1809</v>
       </c>
       <c r="E333" s="20"/>
     </row>
@@ -38571,7 +38780,7 @@
         <v>911</v>
       </c>
       <c r="D334" s="36" t="s">
-        <v>1818</v>
+        <v>1810</v>
       </c>
       <c r="E334" s="20"/>
     </row>
@@ -38586,7 +38795,7 @@
         <v>712</v>
       </c>
       <c r="D335" s="36" t="s">
-        <v>1819</v>
+        <v>1811</v>
       </c>
       <c r="E335" s="20"/>
     </row>
@@ -38601,7 +38810,7 @@
         <v>713</v>
       </c>
       <c r="D336" s="36" t="s">
-        <v>1820</v>
+        <v>1812</v>
       </c>
       <c r="E336" s="20"/>
     </row>
@@ -38616,7 +38825,7 @@
         <v>912</v>
       </c>
       <c r="D337" s="36" t="s">
-        <v>1821</v>
+        <v>1813</v>
       </c>
       <c r="E337" s="20"/>
     </row>
@@ -38631,7 +38840,7 @@
         <v>124</v>
       </c>
       <c r="D338" s="36" t="s">
-        <v>1822</v>
+        <v>1814</v>
       </c>
       <c r="E338" s="20"/>
     </row>
@@ -38646,7 +38855,7 @@
         <v>918</v>
       </c>
       <c r="D339" s="36" t="s">
-        <v>1823</v>
+        <v>1815</v>
       </c>
       <c r="E339" s="20"/>
     </row>
@@ -38658,10 +38867,10 @@
         <v>43038</v>
       </c>
       <c r="C340" s="34" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="D340" s="36" t="s">
-        <v>1824</v>
+        <v>1816</v>
       </c>
       <c r="E340" s="20"/>
     </row>
@@ -38676,7 +38885,7 @@
         <v>716</v>
       </c>
       <c r="D341" s="36" t="s">
-        <v>1825</v>
+        <v>1817</v>
       </c>
       <c r="E341" s="20"/>
     </row>
@@ -38691,7 +38900,7 @@
         <v>126</v>
       </c>
       <c r="D342" s="37" t="s">
-        <v>1826</v>
+        <v>1818</v>
       </c>
       <c r="E342" s="20"/>
     </row>
@@ -38706,7 +38915,7 @@
         <v>984</v>
       </c>
       <c r="D343" s="37" t="s">
-        <v>1827</v>
+        <v>1819</v>
       </c>
       <c r="E343" s="20"/>
     </row>
@@ -38721,7 +38930,7 @@
         <v>170</v>
       </c>
       <c r="D344" s="36" t="s">
-        <v>1828</v>
+        <v>1820</v>
       </c>
       <c r="E344" s="20"/>
     </row>
@@ -38736,7 +38945,7 @@
         <v>718</v>
       </c>
       <c r="D345" s="36" t="s">
-        <v>1829</v>
+        <v>1821</v>
       </c>
       <c r="E345" s="20"/>
     </row>
@@ -38751,7 +38960,7 @@
         <v>917</v>
       </c>
       <c r="D346" s="36" t="s">
-        <v>1830</v>
+        <v>1822</v>
       </c>
       <c r="E346" s="20"/>
     </row>
@@ -38766,7 +38975,7 @@
         <v>920</v>
       </c>
       <c r="D347" s="36" t="s">
-        <v>1831</v>
+        <v>1823</v>
       </c>
       <c r="E347" s="20"/>
     </row>
@@ -38781,7 +38990,7 @@
         <v>127</v>
       </c>
       <c r="D348" s="36" t="s">
-        <v>1832</v>
+        <v>1824</v>
       </c>
       <c r="E348" s="20"/>
     </row>
@@ -38796,7 +39005,7 @@
         <v>719</v>
       </c>
       <c r="D349" s="36" t="s">
-        <v>1833</v>
+        <v>1825</v>
       </c>
       <c r="E349" s="20"/>
     </row>
@@ -38811,7 +39020,7 @@
         <v>171</v>
       </c>
       <c r="D350" s="36" t="s">
-        <v>1834</v>
+        <v>1826</v>
       </c>
       <c r="E350" s="20"/>
     </row>
@@ -38826,7 +39035,7 @@
         <v>128</v>
       </c>
       <c r="D351" s="36" t="s">
-        <v>1835</v>
+        <v>1827</v>
       </c>
       <c r="E351" s="20"/>
     </row>
@@ -38841,7 +39050,7 @@
         <v>129</v>
       </c>
       <c r="D352" s="36" t="s">
-        <v>1836</v>
+        <v>1828</v>
       </c>
       <c r="E352" s="20"/>
     </row>
@@ -38856,7 +39065,7 @@
         <v>916</v>
       </c>
       <c r="D353" s="36" t="s">
-        <v>1837</v>
+        <v>1867</v>
       </c>
       <c r="E353" s="20"/>
     </row>
@@ -38868,10 +39077,10 @@
         <v>43052</v>
       </c>
       <c r="C354" s="34" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="D354" s="36" t="s">
-        <v>1838</v>
+        <v>1829</v>
       </c>
       <c r="E354" s="20"/>
     </row>
@@ -38883,10 +39092,10 @@
         <v>43053</v>
       </c>
       <c r="C355" s="34" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="D355" s="36" t="s">
-        <v>1839</v>
+        <v>1830</v>
       </c>
       <c r="E355" s="20"/>
     </row>
@@ -38901,7 +39110,7 @@
         <v>925</v>
       </c>
       <c r="D356" s="36" t="s">
-        <v>1840</v>
+        <v>1831</v>
       </c>
       <c r="E356" s="20"/>
     </row>
@@ -38916,7 +39125,7 @@
         <v>172</v>
       </c>
       <c r="D357" s="36" t="s">
-        <v>1841</v>
+        <v>1832</v>
       </c>
       <c r="E357" s="20"/>
     </row>
@@ -38931,7 +39140,7 @@
         <v>173</v>
       </c>
       <c r="D358" s="36" t="s">
-        <v>1842</v>
+        <v>1833</v>
       </c>
       <c r="E358" s="20"/>
     </row>
@@ -38946,7 +39155,7 @@
         <v>131</v>
       </c>
       <c r="D359" s="36" t="s">
-        <v>1843</v>
+        <v>1834</v>
       </c>
       <c r="E359" s="20"/>
     </row>
@@ -38961,7 +39170,7 @@
         <v>915</v>
       </c>
       <c r="D360" s="36" t="s">
-        <v>1844</v>
+        <v>1835</v>
       </c>
       <c r="E360" s="20"/>
     </row>
@@ -38976,7 +39185,7 @@
         <v>928</v>
       </c>
       <c r="D361" s="36" t="s">
-        <v>1845</v>
+        <v>1836</v>
       </c>
       <c r="E361" s="20"/>
     </row>
@@ -38991,7 +39200,7 @@
         <v>132</v>
       </c>
       <c r="D362" s="36" t="s">
-        <v>1846</v>
+        <v>1837</v>
       </c>
       <c r="E362" s="20"/>
     </row>
@@ -39006,7 +39215,7 @@
         <v>133</v>
       </c>
       <c r="D363" s="36" t="s">
-        <v>1847</v>
+        <v>1838</v>
       </c>
       <c r="E363" s="20"/>
     </row>
@@ -39021,7 +39230,7 @@
         <v>174</v>
       </c>
       <c r="D364" s="36" t="s">
-        <v>1848</v>
+        <v>1839</v>
       </c>
       <c r="E364" s="20"/>
     </row>
@@ -39036,7 +39245,7 @@
         <v>134</v>
       </c>
       <c r="D365" s="36" t="s">
-        <v>1849</v>
+        <v>1840</v>
       </c>
       <c r="E365" s="20"/>
     </row>
@@ -39051,7 +39260,7 @@
         <v>931</v>
       </c>
       <c r="D366" s="36" t="s">
-        <v>1850</v>
+        <v>1841</v>
       </c>
       <c r="E366" s="20"/>
     </row>
@@ -39066,7 +39275,7 @@
         <v>725</v>
       </c>
       <c r="D367" s="36" t="s">
-        <v>1851</v>
+        <v>1868</v>
       </c>
       <c r="E367" s="20"/>
     </row>
@@ -39081,7 +39290,7 @@
         <v>938</v>
       </c>
       <c r="D368" s="36" t="s">
-        <v>1852</v>
+        <v>1842</v>
       </c>
       <c r="E368" s="20"/>
     </row>
@@ -39096,7 +39305,7 @@
         <v>939</v>
       </c>
       <c r="D369" s="36" t="s">
-        <v>1853</v>
+        <v>1843</v>
       </c>
       <c r="E369" s="20"/>
     </row>
@@ -39111,7 +39320,7 @@
         <v>940</v>
       </c>
       <c r="D370" s="36" t="s">
-        <v>1854</v>
+        <v>1844</v>
       </c>
       <c r="E370" s="20"/>
     </row>
@@ -39126,7 +39335,7 @@
         <v>175</v>
       </c>
       <c r="D371" s="36" t="s">
-        <v>1855</v>
+        <v>1869</v>
       </c>
       <c r="E371" s="20"/>
     </row>
@@ -39141,7 +39350,7 @@
         <v>135</v>
       </c>
       <c r="D372" s="36" t="s">
-        <v>1856</v>
+        <v>1845</v>
       </c>
       <c r="E372" s="20"/>
     </row>
@@ -39156,7 +39365,7 @@
         <v>136</v>
       </c>
       <c r="D373" s="36" t="s">
-        <v>1857</v>
+        <v>1846</v>
       </c>
       <c r="E373" s="20"/>
     </row>

</xml_diff>

<commit_message>
FEAT (Compilation template) Final tweaks
Last pass through the description to correct typos.
</commit_message>
<xml_diff>
--- a/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
+++ b/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="1870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="1871">
   <si>
     <t>Subject</t>
   </si>
@@ -9217,27 +9217,6 @@
     <t>Fourth Sunday of Lent (Mothering Sunday) [1] Violet or Lenten Array</t>
   </si>
   <si>
-    <t>Week of Lent 4
-FOURTH SUNDAY OF LENT [1] Violet or Lenten Array
-MOTHERING SUNDAY
-Exodus 2:1-10 or 1 Samuel 1:20-28
-Psalm 34 or Psalm 127:1-4
-2 Corinthians 1:3-7 or Colossians 3:12-17
-Luke 2:33-35 or John 19:25-27
-DAILY EUCHARIST
-1 Samuel 16:1-13
-Psalm 23
-Ephesians 5:8-14
-John 9:1-41
-DAILY PRAYER: Returning to God 
-Micah 7:1-7, (8-20)
-James 5:1-12, (13-20)
-John 3:14-21
-ALTERNATIVE PSALMS
-Morning: Psalm 31:1-8, (9-16)
-Evening: Psalms 13 and 14</t>
-  </si>
-  <si>
     <t>Holy Week (Week of Lent 6)
 Monday of Holy Week [1] Red or Violet
 (William Law, Priest, 1761 [6] White)
@@ -9348,24 +9327,6 @@
   </si>
   <si>
     <t>John XXIII, Bishop of Rome, Reformer, 1963 [6] White (translated from 4 June)</t>
-  </si>
-  <si>
-    <t>WEEK OF PENTECOST
-Wednesday after the Day of Pentecost (Whitsunday)
-Week of Proper 9 (if after Pentecost) [3] Green
-EMBER DAY READINGS
-isaiah 44:1-8
-Psalm 87
-1 Peter 2:4-10
-John 17:6-19
-DAILY EUCHARIST
-Tobit 3:1-11, 16-17
-Psalm 25:1-8
-Mark 12:18-27
-DAILY PRAYER: Week A
-Deuteronomy 13:1-11
-2 Corinthians 7:2-16
-Luke 17:20-37</t>
   </si>
   <si>
     <t>Saturday after the Day of Pentecost (Whitsunday) / Eve of Trinity Sunday (Ember day)</t>
@@ -10631,26 +10592,6 @@
 Jeremiah 13:1-11
 Romans 6:12-23
 John 8:47-59</t>
-  </si>
-  <si>
-    <t>Holy Week (Week of Lent 6)
-SIXTH SUNDAY: PALM SUNDAY) [1] Red or Violet
-(Dietrich Bonhoeffer, Theologian and Martyr, 1945 [6] Red)
-EUCHARIST
-Liturgy of the Palms
-Matthew 21:1-11
-Psalm 118:1-2, 19-29
-Liturgy of the Passion
-Isaiah 50:4-9a
-Psalm 31:9-16
-Philippians 2:5-11
-Matthew 26:14 - 27:66 or Matthew 27:11-54
-MORNING PRAYER: The Suffering Christ 
-Zechariah 9:9-12
-1 Timothy 6:12-16
-EVENING PRAYER: The Suffering Christ 
-Zechariah 12:9-11; 13:1, 7-9
-Matthew 21:12-17</t>
   </si>
   <si>
     <t>Helena, c.330 [6] White
@@ -13834,6 +13775,83 @@
 Zephaniah 3:1-13
 1 Peter 2:11-25
 Matthew 20:1-16</t>
+  </si>
+  <si>
+    <t>Week of Lent 2
+SECOND SUNDAY OF LENT [1] Violet or Lenten Array
+EUCHARIST
+Genesis 12:1-4a
+Psalm 121
+Romans 4:1-5, 13-17
+John 3:1-17 or Matthew 17:1-9
+DAILY PRAYER: Returning to God 
+Numbers 21:4-9
+Galatians 3:1-9, 23-29
+Luke 14:27-33
+ALTERNATIVE PSALMS
+Morning: Psalm 135:1-14
+Evening: Psalm 74</t>
+  </si>
+  <si>
+    <t>Week of Lent 4
+FOURTH SUNDAY OF LENT [1] Violet or Lenten Array
+DAILY EUCHARIST
+1 Samuel 16:1-13
+Psalm 23
+Ephesians 5:8-14
+John 9:1-41
+DAILY PRAYER: Returning to God 
+Micah 7:1-7, (8-20)
+James 5:1-12, (13-20)
+John 3:14-21
+ALTERNATIVE PSALMS
+Morning: Psalm 31:1-8, (9-16)
+Evening: Psalms 13 and 14
+---
+MOTHERING SUNDAY
+EUCHARIST
+Exodus 2:1-10 or 1 Samuel 1:20-28
+Psalm 34 or Psalm 127:1-4
+2 Corinthians 1:3-7 or Colossians 3:12-17
+Luke 2:33-35 or John 19:25-27</t>
+  </si>
+  <si>
+    <t>Holy Week (Week of Lent 6)
+SIXTH SUNDAY: PALM SUNDAY) [1] Red or Violet
+(Dietrich Bonhoeffer, Theologian and Martyr, 1945 [6] Red)
+EUCHARIST
+Liturgy of the Palms:
+Matthew 21:1-11
+Psalm 118:1-2, 19-29
+Liturgy of the Passion:
+Isaiah 50:4-9a
+Psalm 31:9-16
+Philippians 2:5-11
+Matthew 26:14 - 27:66 or Matthew 27:11-54
+MORNING PRAYER: The Suffering Christ 
+Zechariah 9:9-12
+1 Timothy 6:12-16
+EVENING PRAYER: The Suffering Christ 
+Zechariah 12:9-11; 13:1, 7-9
+Matthew 21:12-17</t>
+  </si>
+  <si>
+    <t>WEEK OF PENTECOST
+Wednesday after the Day of Pentecost (Whitsunday)
+Week of Proper 9 (if after Pentecost) [3] Green
+DAILY EUCHARIST
+Tobit 3:1-11, 16-17
+Psalm 25:1-8
+Mark 12:18-27
+DAILY PRAYER: Week A
+Deuteronomy 13:1-11
+2 Corinthians 7:2-16
+Luke 17:20-37
+EMBER DAY READINGS
+isaiah 44:1-8
+Psalm 87
+1 Peter 2:4-10
+John 17:6-19</t>
   </si>
 </sst>
 </file>
@@ -33958,8 +33976,8 @@
   <dimension ref="A1:E387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D371" sqref="D371"/>
+      <pane ySplit="2" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34004,7 +34022,7 @@
         <v>547</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>1855</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34046,10 +34064,10 @@
         <v>175</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>965</v>
       </c>
@@ -34060,7 +34078,7 @@
         <v>135</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34074,7 +34092,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34088,7 +34106,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34105,7 +34123,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>941</v>
       </c>
@@ -34116,7 +34134,7 @@
         <v>1542</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34130,10 +34148,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>964</v>
       </c>
@@ -34144,7 +34162,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34158,7 +34176,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34242,7 +34260,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34270,7 +34288,7 @@
         <v>556</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -34284,7 +34302,7 @@
         <v>557</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34312,7 +34330,7 @@
         <v>739</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34326,7 +34344,7 @@
         <v>559</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34340,7 +34358,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>1848</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34354,7 +34372,7 @@
         <v>741</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34368,7 +34386,7 @@
         <v>742</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34382,7 +34400,7 @@
         <v>15</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>1849</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34396,7 +34414,7 @@
         <v>16</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>1854</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -34410,7 +34428,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>1850</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -34424,7 +34442,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>1851</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -34438,10 +34456,10 @@
         <v>19</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
         <v>965</v>
       </c>
@@ -34452,7 +34470,7 @@
         <v>20</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34466,7 +34484,7 @@
         <v>137</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34480,7 +34498,7 @@
         <v>21</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -34494,7 +34512,7 @@
         <v>22</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>1857</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34508,7 +34526,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34522,7 +34540,7 @@
         <v>1544</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34536,7 +34554,7 @@
         <v>1545</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34550,7 +34568,7 @@
         <v>1546</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>1858</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34564,7 +34582,7 @@
         <v>24</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>1859</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34575,13 +34593,13 @@
         <v>42742</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
         <v>1519</v>
       </c>
@@ -34620,7 +34638,7 @@
         <v>25</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34634,7 +34652,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34662,10 +34680,10 @@
         <v>138</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="s">
         <v>967</v>
       </c>
@@ -34676,7 +34694,7 @@
         <v>139</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34718,7 +34736,7 @@
         <v>27</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34732,7 +34750,7 @@
         <v>28</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -34774,7 +34792,7 @@
         <v>29</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34816,7 +34834,7 @@
         <v>30</v>
       </c>
       <c r="D61" s="36" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34830,7 +34848,7 @@
         <v>31</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34844,10 +34862,10 @@
         <v>32</v>
       </c>
       <c r="D63" s="36" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="s">
         <v>966</v>
       </c>
@@ -34858,7 +34876,7 @@
         <v>140</v>
       </c>
       <c r="D64" s="36" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34872,7 +34890,7 @@
         <v>33</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -34900,7 +34918,7 @@
         <v>34</v>
       </c>
       <c r="D67" s="36" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -34914,7 +34932,7 @@
         <v>35</v>
       </c>
       <c r="D68" s="36" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -34928,7 +34946,7 @@
         <v>36</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -34942,7 +34960,7 @@
         <v>37</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -34956,10 +34974,10 @@
         <v>141</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="s">
         <v>967</v>
       </c>
@@ -34967,7 +34985,7 @@
         <v>42770</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="D72" s="36" t="s">
         <v>1547</v>
@@ -34987,7 +35005,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
         <v>941</v>
       </c>
@@ -34998,7 +35016,7 @@
         <v>142</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35054,7 +35072,7 @@
         <v>38</v>
       </c>
       <c r="D78" s="36" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35110,7 +35128,7 @@
         <v>39</v>
       </c>
       <c r="D82" s="36" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35124,7 +35142,7 @@
         <v>40</v>
       </c>
       <c r="D83" s="36" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35152,7 +35170,7 @@
         <v>143</v>
       </c>
       <c r="D85" s="36" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35166,7 +35184,7 @@
         <v>41</v>
       </c>
       <c r="D86" s="36" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35183,7 +35201,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A88" s="34" t="s">
         <v>941</v>
       </c>
@@ -35194,7 +35212,7 @@
         <v>1548</v>
       </c>
       <c r="D88" s="37" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35236,7 +35254,7 @@
         <v>43</v>
       </c>
       <c r="D91" s="37" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35267,7 +35285,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A94" s="34" t="s">
         <v>1519</v>
       </c>
@@ -35278,7 +35296,7 @@
         <v>944</v>
       </c>
       <c r="D94" s="37" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35292,7 +35310,7 @@
         <v>796</v>
       </c>
       <c r="D95" s="36" t="s">
-        <v>1860</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35306,7 +35324,7 @@
         <v>582</v>
       </c>
       <c r="D96" s="36" t="s">
-        <v>1861</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35334,10 +35352,10 @@
         <v>144</v>
       </c>
       <c r="D98" s="37" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A99" s="34" t="s">
         <v>966</v>
       </c>
@@ -35348,10 +35366,10 @@
         <v>45</v>
       </c>
       <c r="D99" s="37" t="s">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A100" s="34" t="s">
         <v>967</v>
       </c>
@@ -35362,7 +35380,7 @@
         <v>46</v>
       </c>
       <c r="D100" s="37" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35390,7 +35408,7 @@
         <v>47</v>
       </c>
       <c r="D102" s="36" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35404,7 +35422,7 @@
         <v>48</v>
       </c>
       <c r="D103" s="36" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="285" x14ac:dyDescent="0.25">
@@ -35418,7 +35436,7 @@
         <v>49</v>
       </c>
       <c r="D104" s="36" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35446,7 +35464,7 @@
         <v>50</v>
       </c>
       <c r="D106" s="36" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="300" x14ac:dyDescent="0.25">
@@ -35457,7 +35475,7 @@
         <v>42805</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="D107" s="36" t="s">
         <v>1550</v>
@@ -35474,7 +35492,7 @@
         <v>588</v>
       </c>
       <c r="D108" s="36" t="s">
-        <v>1046</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35530,7 +35548,7 @@
         <v>145</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -35544,10 +35562,10 @@
         <v>146</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A114" s="34" t="s">
         <v>967</v>
       </c>
@@ -35558,7 +35576,7 @@
         <v>147</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -35586,7 +35604,7 @@
         <v>1551</v>
       </c>
       <c r="D116" s="36" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35600,7 +35618,7 @@
         <v>150</v>
       </c>
       <c r="D117" s="36" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35614,10 +35632,10 @@
         <v>151</v>
       </c>
       <c r="D118" s="36" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A119" s="34" t="s">
         <v>965</v>
       </c>
@@ -35628,10 +35646,10 @@
         <v>1552</v>
       </c>
       <c r="D119" s="36" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="285" x14ac:dyDescent="0.25">
       <c r="A120" s="34" t="s">
         <v>966</v>
       </c>
@@ -35642,7 +35660,7 @@
         <v>51</v>
       </c>
       <c r="D120" s="36" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -35656,10 +35674,10 @@
         <v>152</v>
       </c>
       <c r="D121" s="36" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="345" x14ac:dyDescent="0.25">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A122" s="34" t="s">
         <v>1519</v>
       </c>
@@ -35670,7 +35688,7 @@
         <v>1553</v>
       </c>
       <c r="D122" s="36" t="s">
-        <v>1554</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35698,7 +35716,7 @@
         <v>52</v>
       </c>
       <c r="D124" s="36" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35712,7 +35730,7 @@
         <v>544</v>
       </c>
       <c r="D125" s="36" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -35754,10 +35772,10 @@
         <v>153</v>
       </c>
       <c r="D128" s="36" t="s">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A129" s="34" t="s">
         <v>1519</v>
       </c>
@@ -35855,7 +35873,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="330" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="345" x14ac:dyDescent="0.25">
       <c r="A136" s="34" t="s">
         <v>1519</v>
       </c>
@@ -35866,7 +35884,7 @@
         <v>1539</v>
       </c>
       <c r="D136" s="36" t="s">
-        <v>1670</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35880,10 +35898,10 @@
         <v>602</v>
       </c>
       <c r="D137" s="36" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="34" t="s">
         <v>942</v>
       </c>
@@ -35894,7 +35912,7 @@
         <v>603</v>
       </c>
       <c r="D138" s="36" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -35908,7 +35926,7 @@
         <v>604</v>
       </c>
       <c r="D139" s="36" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="195" x14ac:dyDescent="0.25">
@@ -35925,7 +35943,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A141" s="34" t="s">
         <v>966</v>
       </c>
@@ -35953,7 +35971,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A143" s="34" t="s">
         <v>1519</v>
       </c>
@@ -35964,10 +35982,10 @@
         <v>608</v>
       </c>
       <c r="D143" s="36" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A144" s="34" t="s">
         <v>941</v>
       </c>
@@ -35978,7 +35996,7 @@
         <v>609</v>
       </c>
       <c r="D144" s="36" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -36006,7 +36024,7 @@
         <v>611</v>
       </c>
       <c r="D146" s="36" t="s">
-        <v>1862</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="240" x14ac:dyDescent="0.25">
@@ -36020,7 +36038,7 @@
         <v>612</v>
       </c>
       <c r="D147" s="36" t="s">
-        <v>1863</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -36034,7 +36052,7 @@
         <v>613</v>
       </c>
       <c r="D148" s="36" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -36048,10 +36066,10 @@
         <v>614</v>
       </c>
       <c r="D149" s="36" t="s">
-        <v>1865</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A150" s="34" t="s">
         <v>1519</v>
       </c>
@@ -36059,10 +36077,10 @@
         <v>42848</v>
       </c>
       <c r="C150" s="34" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="D150" s="36" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36090,7 +36108,7 @@
         <v>61</v>
       </c>
       <c r="D152" s="37" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -36104,7 +36122,7 @@
         <v>62</v>
       </c>
       <c r="D153" s="37" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36135,7 +36153,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A156" s="34" t="s">
         <v>967</v>
       </c>
@@ -36146,7 +36164,7 @@
         <v>63</v>
       </c>
       <c r="D156" s="37" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -36174,10 +36192,10 @@
         <v>155</v>
       </c>
       <c r="D158" s="37" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A159" s="34" t="s">
         <v>942</v>
       </c>
@@ -36188,7 +36206,7 @@
         <v>1537</v>
       </c>
       <c r="D159" s="37" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36272,7 +36290,7 @@
         <v>156</v>
       </c>
       <c r="D165" s="37" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36317,7 +36335,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A169" s="34" t="s">
         <v>966</v>
       </c>
@@ -36325,10 +36343,10 @@
         <v>42867</v>
       </c>
       <c r="C169" s="34" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="D169" s="37" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36370,7 +36388,7 @@
         <v>65</v>
       </c>
       <c r="D172" s="37" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -36465,10 +36483,10 @@
         <v>42877</v>
       </c>
       <c r="C179" s="34" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D179" s="37" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="285" x14ac:dyDescent="0.25">
@@ -36479,10 +36497,10 @@
         <v>42878</v>
       </c>
       <c r="C180" s="34" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D180" s="37" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="345" x14ac:dyDescent="0.25">
@@ -36493,10 +36511,10 @@
         <v>42879</v>
       </c>
       <c r="C181" s="34" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="D181" s="37" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="195" x14ac:dyDescent="0.25">
@@ -36524,7 +36542,7 @@
         <v>68</v>
       </c>
       <c r="D183" s="37" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="210" x14ac:dyDescent="0.25">
@@ -36535,10 +36553,10 @@
         <v>42882</v>
       </c>
       <c r="C184" s="34" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D184" s="37" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="255" x14ac:dyDescent="0.25">
@@ -36594,7 +36612,7 @@
         <v>69</v>
       </c>
       <c r="D188" s="37" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -36608,7 +36626,7 @@
         <v>158</v>
       </c>
       <c r="D189" s="37" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -36636,7 +36654,7 @@
         <v>70</v>
       </c>
       <c r="D191" s="37" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="240" x14ac:dyDescent="0.25">
@@ -36665,7 +36683,7 @@
         <v>72</v>
       </c>
       <c r="D193" s="36" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="E193" s="20"/>
     </row>
@@ -36677,10 +36695,10 @@
         <v>42892</v>
       </c>
       <c r="C194" s="34" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D194" s="36" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="E194" s="20"/>
     </row>
@@ -36692,10 +36710,10 @@
         <v>42893</v>
       </c>
       <c r="C195" s="34" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="D195" s="36" t="s">
-        <v>1567</v>
+        <v>1870</v>
       </c>
       <c r="E195" s="20"/>
     </row>
@@ -36710,7 +36728,7 @@
         <v>1522</v>
       </c>
       <c r="D196" s="36" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="E196" s="20"/>
     </row>
@@ -36722,10 +36740,10 @@
         <v>42895</v>
       </c>
       <c r="C197" s="41" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D197" s="36" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="E197" s="20"/>
     </row>
@@ -36737,10 +36755,10 @@
         <v>42896</v>
       </c>
       <c r="C198" s="34" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="D198" s="36" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="E198" s="20"/>
     </row>
@@ -36770,7 +36788,7 @@
         <v>74</v>
       </c>
       <c r="D200" s="36" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="E200" s="20"/>
     </row>
@@ -36782,10 +36800,10 @@
         <v>42899</v>
       </c>
       <c r="C201" s="34" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="D201" s="36" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="E201" s="20"/>
     </row>
@@ -36800,7 +36818,7 @@
         <v>76</v>
       </c>
       <c r="D202" s="36" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="E202" s="20"/>
     </row>
@@ -36815,7 +36833,7 @@
         <v>842</v>
       </c>
       <c r="D203" s="24" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="E203" s="20"/>
     </row>
@@ -36830,7 +36848,7 @@
         <v>841</v>
       </c>
       <c r="D204" s="36" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="E204" s="20"/>
     </row>
@@ -36845,7 +36863,7 @@
         <v>645</v>
       </c>
       <c r="D205" s="36" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="E205" s="20"/>
     </row>
@@ -36860,7 +36878,7 @@
         <v>646</v>
       </c>
       <c r="D206" s="36" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="E206" s="20"/>
     </row>
@@ -36872,10 +36890,10 @@
         <v>42905</v>
       </c>
       <c r="C207" s="34" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="D207" s="36" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="E207" s="20"/>
     </row>
@@ -36890,7 +36908,7 @@
         <v>160</v>
       </c>
       <c r="D208" s="36" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
       <c r="E208" s="20"/>
     </row>
@@ -36905,7 +36923,7 @@
         <v>648</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
       <c r="E209" s="20"/>
     </row>
@@ -36920,7 +36938,7 @@
         <v>159</v>
       </c>
       <c r="D210" s="36" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
       <c r="E210" s="20"/>
     </row>
@@ -36935,7 +36953,7 @@
         <v>649</v>
       </c>
       <c r="D211" s="36" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="E211" s="20"/>
     </row>
@@ -36950,7 +36968,7 @@
         <v>78</v>
       </c>
       <c r="D212" s="36" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="E212" s="20"/>
     </row>
@@ -36965,7 +36983,7 @@
         <v>650</v>
       </c>
       <c r="D213" s="36" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="E213" s="20"/>
     </row>
@@ -36980,7 +36998,7 @@
         <v>80</v>
       </c>
       <c r="D214" s="36" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
       <c r="E214" s="20"/>
     </row>
@@ -36995,7 +37013,7 @@
         <v>81</v>
       </c>
       <c r="D215" s="36" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="E215" s="20"/>
     </row>
@@ -37010,7 +37028,7 @@
         <v>82</v>
       </c>
       <c r="D216" s="36" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="E216" s="20"/>
     </row>
@@ -37025,7 +37043,7 @@
         <v>83</v>
       </c>
       <c r="D217" s="36" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="E217" s="20"/>
     </row>
@@ -37037,10 +37055,10 @@
         <v>42916</v>
       </c>
       <c r="C218" s="34" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="D218" s="36" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="E218" s="20"/>
     </row>
@@ -37055,7 +37073,7 @@
         <v>84</v>
       </c>
       <c r="D219" s="36" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="E219" s="20"/>
     </row>
@@ -37070,7 +37088,7 @@
         <v>651</v>
       </c>
       <c r="D220" s="36" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="E220" s="20"/>
     </row>
@@ -37085,7 +37103,7 @@
         <v>85</v>
       </c>
       <c r="D221" s="36" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="E221" s="20"/>
     </row>
@@ -37100,7 +37118,7 @@
         <v>853</v>
       </c>
       <c r="D222" s="36" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="E222" s="20"/>
     </row>
@@ -37115,7 +37133,7 @@
         <v>854</v>
       </c>
       <c r="D223" s="36" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="E223" s="20"/>
     </row>
@@ -37130,7 +37148,7 @@
         <v>161</v>
       </c>
       <c r="D224" s="36" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
       <c r="E224" s="20"/>
     </row>
@@ -37145,7 +37163,7 @@
         <v>97</v>
       </c>
       <c r="D225" s="36" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
       <c r="E225" s="20"/>
     </row>
@@ -37160,7 +37178,7 @@
         <v>653</v>
       </c>
       <c r="D226" s="36" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
       <c r="E226" s="20"/>
     </row>
@@ -37175,7 +37193,7 @@
         <v>654</v>
       </c>
       <c r="D227" s="36" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="E227" s="20"/>
     </row>
@@ -37190,7 +37208,7 @@
         <v>859</v>
       </c>
       <c r="D228" s="36" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="E228" s="20"/>
     </row>
@@ -37205,7 +37223,7 @@
         <v>86</v>
       </c>
       <c r="D229" s="36" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="E229" s="20"/>
     </row>
@@ -37220,7 +37238,7 @@
         <v>87</v>
       </c>
       <c r="D230" s="36" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="E230" s="20"/>
     </row>
@@ -37235,7 +37253,7 @@
         <v>657</v>
       </c>
       <c r="D231" s="36" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="E231" s="20"/>
     </row>
@@ -37250,7 +37268,7 @@
         <v>658</v>
       </c>
       <c r="D232" s="36" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="E232" s="20"/>
     </row>
@@ -37265,7 +37283,7 @@
         <v>860</v>
       </c>
       <c r="D233" s="36" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="E233" s="20"/>
     </row>
@@ -37280,7 +37298,7 @@
         <v>659</v>
       </c>
       <c r="D234" s="36" t="s">
-        <v>1710</v>
+        <v>1707</v>
       </c>
       <c r="E234" s="20"/>
     </row>
@@ -37295,7 +37313,7 @@
         <v>861</v>
       </c>
       <c r="D235" s="36" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="E235" s="20"/>
     </row>
@@ -37310,7 +37328,7 @@
         <v>660</v>
       </c>
       <c r="D236" s="36" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="E236" s="20"/>
     </row>
@@ -37325,7 +37343,7 @@
         <v>661</v>
       </c>
       <c r="D237" s="36" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="E237" s="20"/>
     </row>
@@ -37340,7 +37358,7 @@
         <v>662</v>
       </c>
       <c r="D238" s="36" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="E238" s="20"/>
     </row>
@@ -37355,7 +37373,7 @@
         <v>88</v>
       </c>
       <c r="D239" s="36" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="E239" s="20"/>
     </row>
@@ -37370,7 +37388,7 @@
         <v>89</v>
       </c>
       <c r="D240" s="36" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
       <c r="E240" s="20"/>
     </row>
@@ -37385,7 +37403,7 @@
         <v>665</v>
       </c>
       <c r="D241" s="36" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="E241" s="20"/>
     </row>
@@ -37400,7 +37418,7 @@
         <v>666</v>
       </c>
       <c r="D242" s="36" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="E242" s="20"/>
     </row>
@@ -37415,7 +37433,7 @@
         <v>90</v>
       </c>
       <c r="D243" s="36" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="E243" s="20"/>
     </row>
@@ -37430,7 +37448,7 @@
         <v>91</v>
       </c>
       <c r="D244" s="36" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="E244" s="20"/>
     </row>
@@ -37445,7 +37463,7 @@
         <v>667</v>
       </c>
       <c r="D245" s="36" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="E245" s="20"/>
     </row>
@@ -37460,7 +37478,7 @@
         <v>668</v>
       </c>
       <c r="D246" s="36" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="E246" s="20"/>
     </row>
@@ -37475,7 +37493,7 @@
         <v>92</v>
       </c>
       <c r="D247" s="36" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="E247" s="20"/>
     </row>
@@ -37490,7 +37508,7 @@
         <v>669</v>
       </c>
       <c r="D248" s="36" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="E248" s="20"/>
     </row>
@@ -37505,7 +37523,7 @@
         <v>94</v>
       </c>
       <c r="D249" s="36" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="E249" s="20"/>
     </row>
@@ -37517,10 +37535,10 @@
         <v>42948</v>
       </c>
       <c r="C250" s="34" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="D250" s="36" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="E250" s="20"/>
     </row>
@@ -37535,7 +37553,7 @@
         <v>866</v>
       </c>
       <c r="D251" s="36" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="E251" s="20"/>
     </row>
@@ -37550,7 +37568,7 @@
         <v>867</v>
       </c>
       <c r="D252" s="36" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="E252" s="20"/>
     </row>
@@ -37565,7 +37583,7 @@
         <v>868</v>
       </c>
       <c r="D253" s="36" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="E253" s="20"/>
     </row>
@@ -37580,7 +37598,7 @@
         <v>95</v>
       </c>
       <c r="D254" s="36" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="E254" s="20"/>
     </row>
@@ -37595,7 +37613,7 @@
         <v>96</v>
       </c>
       <c r="D255" s="36" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="E255" s="20"/>
     </row>
@@ -37610,7 +37628,7 @@
         <v>673</v>
       </c>
       <c r="D256" s="36" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="E256" s="20"/>
     </row>
@@ -37625,7 +37643,7 @@
         <v>98</v>
       </c>
       <c r="D257" s="36" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="E257" s="20"/>
     </row>
@@ -37640,7 +37658,7 @@
         <v>99</v>
       </c>
       <c r="D258" s="36" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
       <c r="E258" s="20"/>
     </row>
@@ -37655,7 +37673,7 @@
         <v>162</v>
       </c>
       <c r="D259" s="36" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="E259" s="20"/>
     </row>
@@ -37670,7 +37688,7 @@
         <v>100</v>
       </c>
       <c r="D260" s="36" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="E260" s="20"/>
     </row>
@@ -37685,7 +37703,7 @@
         <v>101</v>
       </c>
       <c r="D261" s="36" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
       <c r="E261" s="20"/>
     </row>
@@ -37700,7 +37718,7 @@
         <v>675</v>
       </c>
       <c r="D262" s="36" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
       <c r="E262" s="20"/>
     </row>
@@ -37715,7 +37733,7 @@
         <v>1538</v>
       </c>
       <c r="D263" s="36" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="E263" s="20"/>
     </row>
@@ -37730,7 +37748,7 @@
         <v>103</v>
       </c>
       <c r="D264" s="36" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="E264" s="20"/>
     </row>
@@ -37742,10 +37760,10 @@
         <v>42963</v>
       </c>
       <c r="C265" s="34" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="D265" s="36" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="E265" s="20"/>
     </row>
@@ -37760,7 +37778,7 @@
         <v>879</v>
       </c>
       <c r="D266" s="36" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="E266" s="20"/>
     </row>
@@ -37775,7 +37793,7 @@
         <v>880</v>
       </c>
       <c r="D267" s="36" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="E267" s="20"/>
     </row>
@@ -37790,7 +37808,7 @@
         <v>881</v>
       </c>
       <c r="D268" s="36" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="E268" s="20"/>
     </row>
@@ -37805,7 +37823,7 @@
         <v>676</v>
       </c>
       <c r="D269" s="36" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="E269" s="20"/>
     </row>
@@ -37820,7 +37838,7 @@
         <v>1530</v>
       </c>
       <c r="D270" s="36" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
       <c r="E270" s="20"/>
     </row>
@@ -37835,7 +37853,7 @@
         <v>678</v>
       </c>
       <c r="D271" s="36" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="E271" s="20"/>
     </row>
@@ -37850,7 +37868,7 @@
         <v>679</v>
       </c>
       <c r="D272" s="36" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="E272" s="20"/>
     </row>
@@ -37865,7 +37883,7 @@
         <v>163</v>
       </c>
       <c r="D273" s="36" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="E273" s="20"/>
     </row>
@@ -37880,7 +37898,7 @@
         <v>164</v>
       </c>
       <c r="D274" s="36" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="E274" s="20"/>
     </row>
@@ -37895,7 +37913,7 @@
         <v>681</v>
       </c>
       <c r="D275" s="36" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="E275" s="20"/>
     </row>
@@ -37910,7 +37928,7 @@
         <v>682</v>
       </c>
       <c r="D276" s="36" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="E276" s="20"/>
     </row>
@@ -37925,7 +37943,7 @@
         <v>165</v>
       </c>
       <c r="D277" s="36" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="E277" s="20"/>
     </row>
@@ -37940,7 +37958,7 @@
         <v>105</v>
       </c>
       <c r="D278" s="36" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="E278" s="20"/>
     </row>
@@ -37952,10 +37970,10 @@
         <v>42977</v>
       </c>
       <c r="C279" s="34" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="D279" s="36" t="s">
-        <v>1755</v>
+        <v>1752</v>
       </c>
       <c r="E279" s="20"/>
     </row>
@@ -37970,7 +37988,7 @@
         <v>106</v>
       </c>
       <c r="D280" s="36" t="s">
-        <v>1756</v>
+        <v>1753</v>
       </c>
       <c r="E280" s="20"/>
     </row>
@@ -37985,7 +38003,7 @@
         <v>886</v>
       </c>
       <c r="D281" s="36" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="E281" s="20"/>
     </row>
@@ -38000,7 +38018,7 @@
         <v>107</v>
       </c>
       <c r="D282" s="36" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="E282" s="20"/>
     </row>
@@ -38015,7 +38033,7 @@
         <v>684</v>
       </c>
       <c r="D283" s="36" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="E283" s="20"/>
     </row>
@@ -38030,7 +38048,7 @@
         <v>108</v>
       </c>
       <c r="D284" s="36" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
       <c r="E284" s="20"/>
     </row>
@@ -38045,7 +38063,7 @@
         <v>685</v>
       </c>
       <c r="D285" s="36" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="E285" s="20"/>
     </row>
@@ -38060,7 +38078,7 @@
         <v>889</v>
       </c>
       <c r="D286" s="36" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="E286" s="20"/>
     </row>
@@ -38075,7 +38093,7 @@
         <v>890</v>
       </c>
       <c r="D287" s="36" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="E287" s="20"/>
     </row>
@@ -38090,7 +38108,7 @@
         <v>109</v>
       </c>
       <c r="D288" s="36" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="E288" s="20"/>
     </row>
@@ -38105,7 +38123,7 @@
         <v>687</v>
       </c>
       <c r="D289" s="36" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="E289" s="20"/>
     </row>
@@ -38120,7 +38138,7 @@
         <v>688</v>
       </c>
       <c r="D290" s="36" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="E290" s="20"/>
     </row>
@@ -38135,7 +38153,7 @@
         <v>689</v>
       </c>
       <c r="D291" s="36" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="E291" s="20"/>
     </row>
@@ -38150,7 +38168,7 @@
         <v>891</v>
       </c>
       <c r="D292" s="36" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="E292" s="20"/>
     </row>
@@ -38165,7 +38183,7 @@
         <v>110</v>
       </c>
       <c r="D293" s="36" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="E293" s="20"/>
     </row>
@@ -38180,7 +38198,7 @@
         <v>166</v>
       </c>
       <c r="D294" s="36" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="E294" s="20"/>
     </row>
@@ -38195,7 +38213,7 @@
         <v>692</v>
       </c>
       <c r="D295" s="36" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="E295" s="20"/>
     </row>
@@ -38210,7 +38228,7 @@
         <v>111</v>
       </c>
       <c r="D296" s="36" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="E296" s="20"/>
     </row>
@@ -38225,7 +38243,7 @@
         <v>694</v>
       </c>
       <c r="D297" s="36" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="E297" s="20"/>
     </row>
@@ -38240,7 +38258,7 @@
         <v>112</v>
       </c>
       <c r="D298" s="36" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="E298" s="20"/>
     </row>
@@ -38255,7 +38273,7 @@
         <v>893</v>
       </c>
       <c r="D299" s="36" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="E299" s="20"/>
     </row>
@@ -38270,7 +38288,7 @@
         <v>113</v>
       </c>
       <c r="D300" s="36" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="E300" s="20"/>
     </row>
@@ -38285,7 +38303,7 @@
         <v>167</v>
       </c>
       <c r="D301" s="36" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="E301" s="20"/>
     </row>
@@ -38297,10 +38315,10 @@
         <v>43000</v>
       </c>
       <c r="C302" s="34" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="D302" s="36" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="E302" s="20"/>
     </row>
@@ -38312,10 +38330,10 @@
         <v>43001</v>
       </c>
       <c r="C303" s="34" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="D303" s="36" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="E303" s="20"/>
     </row>
@@ -38330,7 +38348,7 @@
         <v>697</v>
       </c>
       <c r="D304" s="36" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="E304" s="20"/>
     </row>
@@ -38345,7 +38363,7 @@
         <v>176</v>
       </c>
       <c r="D305" s="36" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="E305" s="20"/>
     </row>
@@ -38360,7 +38378,7 @@
         <v>897</v>
       </c>
       <c r="D306" s="36" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
       <c r="E306" s="20"/>
     </row>
@@ -38375,7 +38393,7 @@
         <v>115</v>
       </c>
       <c r="D307" s="36" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="E307" s="20"/>
     </row>
@@ -38390,7 +38408,7 @@
         <v>698</v>
       </c>
       <c r="D308" s="36" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="E308" s="20"/>
     </row>
@@ -38405,7 +38423,7 @@
         <v>116</v>
       </c>
       <c r="D309" s="36" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="E309" s="20"/>
     </row>
@@ -38420,7 +38438,7 @@
         <v>117</v>
       </c>
       <c r="D310" s="36" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="E310" s="20"/>
     </row>
@@ -38435,7 +38453,7 @@
         <v>700</v>
       </c>
       <c r="D311" s="36" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="E311" s="20"/>
     </row>
@@ -38447,10 +38465,10 @@
         <v>43010</v>
       </c>
       <c r="C312" s="34" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="D312" s="36" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="E312" s="20"/>
     </row>
@@ -38465,7 +38483,7 @@
         <v>901</v>
       </c>
       <c r="D313" s="36" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="E313" s="20"/>
     </row>
@@ -38480,7 +38498,7 @@
         <v>119</v>
       </c>
       <c r="D314" s="36" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="E314" s="20"/>
     </row>
@@ -38495,7 +38513,7 @@
         <v>903</v>
       </c>
       <c r="D315" s="36" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="E315" s="20"/>
     </row>
@@ -38510,7 +38528,7 @@
         <v>701</v>
       </c>
       <c r="D316" s="36" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="E316" s="20"/>
     </row>
@@ -38525,7 +38543,7 @@
         <v>702</v>
       </c>
       <c r="D317" s="36" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="E317" s="20"/>
     </row>
@@ -38537,10 +38555,10 @@
         <v>43016</v>
       </c>
       <c r="C318" s="34" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="D318" s="36" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="E318" s="20"/>
     </row>
@@ -38552,10 +38570,10 @@
         <v>43017</v>
       </c>
       <c r="C319" s="34" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="D319" s="36" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="E319" s="20"/>
     </row>
@@ -38570,7 +38588,7 @@
         <v>704</v>
       </c>
       <c r="D320" s="36" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="E320" s="20"/>
     </row>
@@ -38585,7 +38603,7 @@
         <v>120</v>
       </c>
       <c r="D321" s="36" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="E321" s="20"/>
     </row>
@@ -38600,7 +38618,7 @@
         <v>168</v>
       </c>
       <c r="D322" s="36" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="E322" s="20"/>
     </row>
@@ -38612,10 +38630,10 @@
         <v>43021</v>
       </c>
       <c r="C323" s="34" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="D323" s="36" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="E323" s="20"/>
     </row>
@@ -38630,7 +38648,7 @@
         <v>707</v>
       </c>
       <c r="D324" s="36" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="E324" s="20"/>
     </row>
@@ -38645,7 +38663,7 @@
         <v>708</v>
       </c>
       <c r="D325" s="36" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="E325" s="20"/>
     </row>
@@ -38657,10 +38675,10 @@
         <v>43024</v>
       </c>
       <c r="C326" s="34" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="D326" s="36" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="E326" s="20"/>
     </row>
@@ -38675,7 +38693,7 @@
         <v>122</v>
       </c>
       <c r="D327" s="36" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="E327" s="20"/>
     </row>
@@ -38690,7 +38708,7 @@
         <v>123</v>
       </c>
       <c r="D328" s="36" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="E328" s="20"/>
     </row>
@@ -38705,7 +38723,7 @@
         <v>169</v>
       </c>
       <c r="D329" s="36" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="E329" s="20"/>
     </row>
@@ -38720,7 +38738,7 @@
         <v>710</v>
       </c>
       <c r="D330" s="36" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="E330" s="20"/>
     </row>
@@ -38735,7 +38753,7 @@
         <v>909</v>
       </c>
       <c r="D331" s="36" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="E331" s="20"/>
     </row>
@@ -38750,7 +38768,7 @@
         <v>711</v>
       </c>
       <c r="D332" s="36" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="E332" s="20"/>
     </row>
@@ -38765,7 +38783,7 @@
         <v>1527</v>
       </c>
       <c r="D333" s="36" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="E333" s="20"/>
     </row>
@@ -38780,7 +38798,7 @@
         <v>911</v>
       </c>
       <c r="D334" s="36" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="E334" s="20"/>
     </row>
@@ -38795,7 +38813,7 @@
         <v>712</v>
       </c>
       <c r="D335" s="36" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="E335" s="20"/>
     </row>
@@ -38810,7 +38828,7 @@
         <v>713</v>
       </c>
       <c r="D336" s="36" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="E336" s="20"/>
     </row>
@@ -38825,7 +38843,7 @@
         <v>912</v>
       </c>
       <c r="D337" s="36" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="E337" s="20"/>
     </row>
@@ -38840,7 +38858,7 @@
         <v>124</v>
       </c>
       <c r="D338" s="36" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="E338" s="20"/>
     </row>
@@ -38855,7 +38873,7 @@
         <v>918</v>
       </c>
       <c r="D339" s="36" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="E339" s="20"/>
     </row>
@@ -38867,10 +38885,10 @@
         <v>43038</v>
       </c>
       <c r="C340" s="34" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="D340" s="36" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="E340" s="20"/>
     </row>
@@ -38885,7 +38903,7 @@
         <v>716</v>
       </c>
       <c r="D341" s="36" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="E341" s="20"/>
     </row>
@@ -38900,7 +38918,7 @@
         <v>126</v>
       </c>
       <c r="D342" s="37" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="E342" s="20"/>
     </row>
@@ -38915,7 +38933,7 @@
         <v>984</v>
       </c>
       <c r="D343" s="37" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="E343" s="20"/>
     </row>
@@ -38930,7 +38948,7 @@
         <v>170</v>
       </c>
       <c r="D344" s="36" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
       <c r="E344" s="20"/>
     </row>
@@ -38945,7 +38963,7 @@
         <v>718</v>
       </c>
       <c r="D345" s="36" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="E345" s="20"/>
     </row>
@@ -38960,7 +38978,7 @@
         <v>917</v>
       </c>
       <c r="D346" s="36" t="s">
-        <v>1822</v>
+        <v>1819</v>
       </c>
       <c r="E346" s="20"/>
     </row>
@@ -38975,7 +38993,7 @@
         <v>920</v>
       </c>
       <c r="D347" s="36" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="E347" s="20"/>
     </row>
@@ -38990,7 +39008,7 @@
         <v>127</v>
       </c>
       <c r="D348" s="36" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
       <c r="E348" s="20"/>
     </row>
@@ -39005,7 +39023,7 @@
         <v>719</v>
       </c>
       <c r="D349" s="36" t="s">
-        <v>1825</v>
+        <v>1822</v>
       </c>
       <c r="E349" s="20"/>
     </row>
@@ -39020,7 +39038,7 @@
         <v>171</v>
       </c>
       <c r="D350" s="36" t="s">
-        <v>1826</v>
+        <v>1823</v>
       </c>
       <c r="E350" s="20"/>
     </row>
@@ -39035,7 +39053,7 @@
         <v>128</v>
       </c>
       <c r="D351" s="36" t="s">
-        <v>1827</v>
+        <v>1824</v>
       </c>
       <c r="E351" s="20"/>
     </row>
@@ -39050,7 +39068,7 @@
         <v>129</v>
       </c>
       <c r="D352" s="36" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
       <c r="E352" s="20"/>
     </row>
@@ -39065,7 +39083,7 @@
         <v>916</v>
       </c>
       <c r="D353" s="36" t="s">
-        <v>1867</v>
+        <v>1864</v>
       </c>
       <c r="E353" s="20"/>
     </row>
@@ -39077,10 +39095,10 @@
         <v>43052</v>
       </c>
       <c r="C354" s="34" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D354" s="36" t="s">
-        <v>1829</v>
+        <v>1826</v>
       </c>
       <c r="E354" s="20"/>
     </row>
@@ -39092,10 +39110,10 @@
         <v>43053</v>
       </c>
       <c r="C355" s="34" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="D355" s="36" t="s">
-        <v>1830</v>
+        <v>1827</v>
       </c>
       <c r="E355" s="20"/>
     </row>
@@ -39110,7 +39128,7 @@
         <v>925</v>
       </c>
       <c r="D356" s="36" t="s">
-        <v>1831</v>
+        <v>1828</v>
       </c>
       <c r="E356" s="20"/>
     </row>
@@ -39125,7 +39143,7 @@
         <v>172</v>
       </c>
       <c r="D357" s="36" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="E357" s="20"/>
     </row>
@@ -39140,7 +39158,7 @@
         <v>173</v>
       </c>
       <c r="D358" s="36" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
       <c r="E358" s="20"/>
     </row>
@@ -39155,7 +39173,7 @@
         <v>131</v>
       </c>
       <c r="D359" s="36" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
       <c r="E359" s="20"/>
     </row>
@@ -39170,7 +39188,7 @@
         <v>915</v>
       </c>
       <c r="D360" s="36" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="E360" s="20"/>
     </row>
@@ -39185,7 +39203,7 @@
         <v>928</v>
       </c>
       <c r="D361" s="36" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
       <c r="E361" s="20"/>
     </row>
@@ -39200,7 +39218,7 @@
         <v>132</v>
       </c>
       <c r="D362" s="36" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="E362" s="20"/>
     </row>
@@ -39215,7 +39233,7 @@
         <v>133</v>
       </c>
       <c r="D363" s="36" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="E363" s="20"/>
     </row>
@@ -39230,7 +39248,7 @@
         <v>174</v>
       </c>
       <c r="D364" s="36" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="E364" s="20"/>
     </row>
@@ -39245,7 +39263,7 @@
         <v>134</v>
       </c>
       <c r="D365" s="36" t="s">
-        <v>1840</v>
+        <v>1837</v>
       </c>
       <c r="E365" s="20"/>
     </row>
@@ -39260,7 +39278,7 @@
         <v>931</v>
       </c>
       <c r="D366" s="36" t="s">
-        <v>1841</v>
+        <v>1838</v>
       </c>
       <c r="E366" s="20"/>
     </row>
@@ -39275,7 +39293,7 @@
         <v>725</v>
       </c>
       <c r="D367" s="36" t="s">
-        <v>1868</v>
+        <v>1865</v>
       </c>
       <c r="E367" s="20"/>
     </row>
@@ -39290,7 +39308,7 @@
         <v>938</v>
       </c>
       <c r="D368" s="36" t="s">
-        <v>1842</v>
+        <v>1839</v>
       </c>
       <c r="E368" s="20"/>
     </row>
@@ -39305,7 +39323,7 @@
         <v>939</v>
       </c>
       <c r="D369" s="36" t="s">
-        <v>1843</v>
+        <v>1840</v>
       </c>
       <c r="E369" s="20"/>
     </row>
@@ -39320,7 +39338,7 @@
         <v>940</v>
       </c>
       <c r="D370" s="36" t="s">
-        <v>1844</v>
+        <v>1841</v>
       </c>
       <c r="E370" s="20"/>
     </row>
@@ -39335,7 +39353,7 @@
         <v>175</v>
       </c>
       <c r="D371" s="36" t="s">
-        <v>1869</v>
+        <v>1866</v>
       </c>
       <c r="E371" s="20"/>
     </row>
@@ -39350,7 +39368,7 @@
         <v>135</v>
       </c>
       <c r="D372" s="36" t="s">
-        <v>1845</v>
+        <v>1842</v>
       </c>
       <c r="E372" s="20"/>
     </row>
@@ -39365,7 +39383,7 @@
         <v>136</v>
       </c>
       <c r="D373" s="36" t="s">
-        <v>1846</v>
+        <v>1843</v>
       </c>
       <c r="E373" s="20"/>
     </row>

</xml_diff>

<commit_message>
FIX (2016-2017) Fix typo
Fix typo in name of Sixth Sunday of Lent (was 'Sxith')
</commit_message>
<xml_diff>
--- a/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
+++ b/2016-2017 A1/sec-master-calendar-2016-2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4894" uniqueCount="1873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4894" uniqueCount="1874">
   <si>
     <t>Subject</t>
   </si>
@@ -13903,6 +13903,9 @@
 Colossians 2:6-12
 John 16:23b-30
 Happy new year! Lang may yer lum reek!</t>
+  </si>
+  <si>
+    <t>Sixth Sunday of Lent (Palm Sunday: The beginning of Holy Week) [1] Red or Violet</t>
   </si>
 </sst>
 </file>
@@ -15369,8 +15372,8 @@
   </sheetPr>
   <dimension ref="A1:K372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17710,7 +17713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A90" s="36" t="s">
         <v>43</v>
       </c>
@@ -17762,7 +17765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A92" s="36" t="s">
         <v>779</v>
       </c>
@@ -18882,7 +18885,7 @@
     </row>
     <row r="135" spans="1:11" ht="375" x14ac:dyDescent="0.25">
       <c r="A135" s="36" t="s">
-        <v>1539</v>
+        <v>1873</v>
       </c>
       <c r="B135" s="33">
         <v>42834</v>
@@ -18984,7 +18987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A139" s="36" t="s">
         <v>605</v>
       </c>
@@ -20024,7 +20027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="300" x14ac:dyDescent="0.25">
       <c r="A179" s="36" t="s">
         <v>1562</v>
       </c>
@@ -20128,7 +20131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A183" s="36" t="s">
         <v>1564</v>
       </c>

</xml_diff>